<commit_message>
Including predation losses and gains
Signed-off-by: Guillaume Daudin <gdaudin@mac.com>
</commit_message>
<xml_diff>
--- a/External Data/Résultats de la course française.xlsx
+++ b/External Data/Résultats de la course française.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumedaudin/Répertoires GIT/2016-Hamburg-Impact-of-War/External Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumedaudin/Répertoires Git/2016-Hamburg-Impact-of-War/External Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC66A508-E8B7-FF40-A480-35415D5373EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECE3BB8-8C7E-2E48-AAD5-53F39B26D71B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38040" yWindow="2400" windowWidth="28040" windowHeight="16860" xr2:uid="{E3D52932-A783-EC49-8617-8937D12F747E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{E3D52932-A783-EC49-8617-8937D12F747E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Calcul" sheetId="1" r:id="rId1"/>
+    <sheet name="Output" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
   <si>
     <t>Estimation de l’armement corsaire à Dunkerque, Saint-Malo et Bayonne (en milliers de lt) Villier 2002, p. 327</t>
   </si>
@@ -179,6 +178,45 @@
   </si>
   <si>
     <t>Roll of English Merchant-Vessels captured by the French during the War</t>
+  </si>
+  <si>
+    <t>Crowhurst par Acerra Meyer "Appendice 1 Marine et Révolution"</t>
+  </si>
+  <si>
+    <t>Nombre d’armements (?)</t>
+  </si>
+  <si>
+    <t>Dukerque guerre d’Amérique : 198 armements (voir Villiers p. 670) pour 19 M d’investissement.</t>
+  </si>
+  <si>
+    <t>Armement moyen :</t>
+  </si>
+  <si>
+    <t>Investissement Villiers / Crowhurst</t>
+  </si>
+  <si>
+    <t>Prises en utilisant le ratio de la guerre d’Amérpque</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeur par prise : </t>
+  </si>
+  <si>
+    <t>Prises en utilisant Normann</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>French investment</t>
+  </si>
+  <si>
+    <t>Part de captures privées</t>
+  </si>
+  <si>
+    <t>Ivestissement en utilisant Normann (que pour course privée)</t>
+  </si>
+  <si>
+    <t>French income</t>
   </si>
 </sst>
 </file>
@@ -539,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747C72A1-6A8D-9E42-88DE-481B3F912E70}">
-  <dimension ref="A1:L190"/>
+  <dimension ref="A1:L231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="A188" sqref="A188"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1582,11 +1620,11 @@
         <v>1756</v>
       </c>
       <c r="B94" s="1">
-        <f>B68*E79/E54</f>
+        <f t="shared" ref="B94:B100" si="13">B68*E79/E54</f>
         <v>7697.7600927145941</v>
       </c>
       <c r="C94" s="2">
-        <f>B94/B68</f>
+        <f t="shared" ref="C94:C101" si="14">B94/B68</f>
         <v>2.2771483264640833</v>
       </c>
       <c r="D94" s="1">
@@ -1599,7 +1637,7 @@
         <v>1757</v>
       </c>
       <c r="B95" s="1">
-        <f>B69*E80/E55</f>
+        <f t="shared" si="13"/>
         <v>10493.906116551223</v>
       </c>
       <c r="C95" s="2">
@@ -1607,7 +1645,7 @@
         <v>0.98733895649953818</v>
       </c>
       <c r="D95" s="1">
-        <f t="shared" ref="D95:D100" si="13">$A$104*B95/$B$101</f>
+        <f t="shared" ref="D95:D100" si="15">$A$104*B95/$B$101</f>
         <v>1698.1346656424962</v>
       </c>
     </row>
@@ -1616,15 +1654,15 @@
         <v>1758</v>
       </c>
       <c r="B96" s="1">
-        <f>B70*E81/E56</f>
+        <f t="shared" si="13"/>
         <v>5847.2293417575765</v>
       </c>
       <c r="C96" s="2">
-        <f>B96/B70</f>
+        <f t="shared" si="14"/>
         <v>1.0262687714355536</v>
       </c>
       <c r="D96" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>946.20465753354233</v>
       </c>
     </row>
@@ -1633,15 +1671,15 @@
         <v>1759</v>
       </c>
       <c r="B97" s="1">
-        <f>B71*E82/E57</f>
+        <f t="shared" si="13"/>
         <v>6808.6733157894741</v>
       </c>
       <c r="C97" s="2">
-        <f>B97/B71</f>
+        <f t="shared" si="14"/>
         <v>2.3815461496450028</v>
       </c>
       <c r="D97" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1101.7865088712038</v>
       </c>
     </row>
@@ -1650,15 +1688,15 @@
         <v>1760</v>
       </c>
       <c r="B98" s="1">
-        <f>B72*E83/E58</f>
+        <f t="shared" si="13"/>
         <v>13751.472459119865</v>
       </c>
       <c r="C98" s="2">
-        <f>B98/B72</f>
+        <f t="shared" si="14"/>
         <v>3.9996016398260634</v>
       </c>
       <c r="D98" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2225.2773969102354</v>
       </c>
     </row>
@@ -1667,15 +1705,15 @@
         <v>1761</v>
       </c>
       <c r="B99" s="1">
-        <f>B73*E84/E59</f>
+        <f t="shared" si="13"/>
         <v>6688.8031702564049</v>
       </c>
       <c r="C99" s="2">
-        <f>B99/B73</f>
+        <f t="shared" si="14"/>
         <v>2.1635556730485477</v>
       </c>
       <c r="D99" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1082.3889988073142</v>
       </c>
     </row>
@@ -1684,15 +1722,15 @@
         <v>1762</v>
       </c>
       <c r="B100" s="1">
-        <f>B74*E85/E60</f>
+        <f t="shared" si="13"/>
         <v>4329.1551209921654</v>
       </c>
       <c r="C100" s="2">
-        <f>B100/B74</f>
+        <f t="shared" si="14"/>
         <v>1.2441574894008587</v>
       </c>
       <c r="D100" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>700.54832797728193</v>
       </c>
     </row>
@@ -1702,7 +1740,7 @@
         <v>55616.999617181304</v>
       </c>
       <c r="C101" s="2">
-        <f>B101/B75</f>
+        <f t="shared" si="14"/>
         <v>1.7073637464023181</v>
       </c>
       <c r="D101" s="1">
@@ -1894,7 +1932,7 @@
         <v>1779</v>
       </c>
       <c r="B131" s="1">
-        <f t="shared" ref="B131:B135" si="14">B123/$B$128*$A$108</f>
+        <f t="shared" ref="B131:B135" si="16">B123/$B$128*$A$108</f>
         <v>5858.5858585858587</v>
       </c>
     </row>
@@ -1903,7 +1941,7 @@
         <v>1780</v>
       </c>
       <c r="B132" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>9292.9292929292933</v>
       </c>
     </row>
@@ -1912,7 +1950,7 @@
         <v>1781</v>
       </c>
       <c r="B133" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>9494.9494949494947</v>
       </c>
     </row>
@@ -1921,7 +1959,7 @@
         <v>1782</v>
       </c>
       <c r="B134" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>10707.070707070707</v>
       </c>
     </row>
@@ -1930,8 +1968,14 @@
         <v>1783</v>
       </c>
       <c r="B135" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>606.06060606060612</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B136" s="1">
+        <f>SUM(B130:B135)</f>
+        <v>40000</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
@@ -1953,7 +1997,7 @@
         <v>1779</v>
       </c>
       <c r="B139" s="1">
-        <f t="shared" ref="B139:B143" si="15">B123/$B$128*$B$119</f>
+        <f t="shared" ref="B139:B143" si="17">B123/$B$128*$B$119</f>
         <v>4086.8564641655207</v>
       </c>
     </row>
@@ -1962,7 +2006,7 @@
         <v>1780</v>
       </c>
       <c r="B140" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6482.5999086763431</v>
       </c>
     </row>
@@ -1971,7 +2015,7 @@
         <v>1781</v>
       </c>
       <c r="B141" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6623.5259936475677</v>
       </c>
     </row>
@@ -1980,7 +2024,7 @@
         <v>1782</v>
       </c>
       <c r="B142" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>7469.0825034749168</v>
       </c>
     </row>
@@ -1989,7 +2033,7 @@
         <v>1783</v>
       </c>
       <c r="B143" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>422.77825491367457</v>
       </c>
     </row>
@@ -2072,7 +2116,7 @@
         <v>1779</v>
       </c>
       <c r="B157" s="1">
-        <f t="shared" ref="B157:B161" si="16">$A$110/$B$153*B148</f>
+        <f t="shared" ref="B157:B161" si="18">$A$110/$B$153*B148</f>
         <v>4761.2156295224313</v>
       </c>
     </row>
@@ -2081,7 +2125,7 @@
         <v>1780</v>
       </c>
       <c r="B158" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5774.2402315484806</v>
       </c>
     </row>
@@ -2090,7 +2134,7 @@
         <v>1781</v>
       </c>
       <c r="B159" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>9876.9898697539793</v>
       </c>
     </row>
@@ -2099,37 +2143,44 @@
         <v>1782</v>
       </c>
       <c r="B160" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3494.9348769898697</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>1783</v>
       </c>
       <c r="B161" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>202.60492040520984</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D161" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B162" s="1">
         <f>SUM(B156:B161)</f>
         <v>35000</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D162" s="2">
+        <f>B136/(B136+B162)</f>
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>1793</v>
       </c>
@@ -2137,7 +2188,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>1794</v>
       </c>
@@ -2145,7 +2196,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>1795</v>
       </c>
@@ -2153,7 +2204,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>1796</v>
       </c>
@@ -2161,7 +2212,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>1797</v>
       </c>
@@ -2169,7 +2220,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>1798</v>
       </c>
@@ -2177,7 +2228,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>1799</v>
       </c>
@@ -2185,7 +2236,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>1800</v>
       </c>
@@ -2303,10 +2354,1163 @@
       </c>
       <c r="B190" s="1">
         <v>145</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B194" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" s="1">
+        <v>1793</v>
+      </c>
+      <c r="B195" s="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" s="1">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" s="1">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" s="1">
+        <v>1796</v>
+      </c>
+      <c r="B198" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" s="1">
+        <v>1797</v>
+      </c>
+      <c r="B199" s="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" s="1">
+        <v>1798</v>
+      </c>
+      <c r="B200" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" s="1">
+        <v>1799</v>
+      </c>
+      <c r="B201" s="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" s="1">
+        <v>1800</v>
+      </c>
+      <c r="B202" s="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" s="1">
+        <v>1801</v>
+      </c>
+      <c r="B203" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D206" s="1">
+        <f>19000/198</f>
+        <v>95.959595959595958</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B209" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H209" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I209" s="1">
+        <f>SUM(C210:C218)/(SUM(B169:B177)-B170-B171)</f>
+        <v>24.225126676157274</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A210" s="1">
+        <v>1793</v>
+      </c>
+      <c r="B210" s="1">
+        <f>B195*$D$206</f>
+        <v>12666.666666666666</v>
+      </c>
+      <c r="C210" s="1">
+        <f>B210*$C$119</f>
+        <v>18157.90568115942</v>
+      </c>
+      <c r="D210" s="1">
+        <f>B169*$I$209</f>
+        <v>8527.2445900073599</v>
+      </c>
+      <c r="E210" s="1">
+        <f>D210/$C$119*$D$162</f>
+        <v>3172.5175565471377</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A211" s="1">
+        <v>1794</v>
+      </c>
+      <c r="D211" s="1">
+        <f t="shared" ref="D211:D238" si="19">B170*$I$209</f>
+        <v>15600.981579445284</v>
+      </c>
+      <c r="E211" s="1">
+        <f t="shared" ref="E211:E231" si="20">D211/$C$119*$D$162</f>
+        <v>5804.2650750464682</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A212" s="1">
+        <v>1795</v>
+      </c>
+      <c r="D212" s="1">
+        <f t="shared" si="19"/>
+        <v>15504.081072740655</v>
+      </c>
+      <c r="E212" s="1">
+        <f t="shared" si="20"/>
+        <v>5768.2137391766146</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A213" s="1">
+        <v>1796</v>
+      </c>
+      <c r="B213" s="1">
+        <f t="shared" ref="B211:B218" si="21">B198*$D$206</f>
+        <v>4318.181818181818</v>
+      </c>
+      <c r="C213" s="1">
+        <f>B213*1.5</f>
+        <v>6477.272727272727</v>
+      </c>
+      <c r="D213" s="1">
+        <f t="shared" si="19"/>
+        <v>11846.086944640907</v>
+      </c>
+      <c r="E213" s="1">
+        <f t="shared" si="20"/>
+        <v>4407.2758100896317</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A214" s="1">
+        <v>1797</v>
+      </c>
+      <c r="B214" s="1">
+        <f t="shared" si="21"/>
+        <v>13914.141414141413</v>
+      </c>
+      <c r="C214" s="1">
+        <f t="shared" ref="C214:C218" si="22">B214*1.5</f>
+        <v>20871.21212121212</v>
+      </c>
+      <c r="D214" s="1">
+        <f t="shared" si="19"/>
+        <v>22989.645215673252</v>
+      </c>
+      <c r="E214" s="1">
+        <f t="shared" si="20"/>
+        <v>8553.1794351228236</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A215" s="1">
+        <v>1798</v>
+      </c>
+      <c r="B215" s="1">
+        <f t="shared" si="21"/>
+        <v>13818.181818181818</v>
+      </c>
+      <c r="C215" s="1">
+        <f t="shared" si="22"/>
+        <v>20727.272727272728</v>
+      </c>
+      <c r="D215" s="1">
+        <f t="shared" si="19"/>
+        <v>16666.887153196203</v>
+      </c>
+      <c r="E215" s="1">
+        <f t="shared" si="20"/>
+        <v>6200.8297696148602</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A216" s="1">
+        <v>1799</v>
+      </c>
+      <c r="B216" s="1">
+        <f t="shared" si="21"/>
+        <v>11227.272727272728</v>
+      </c>
+      <c r="C216" s="1">
+        <f t="shared" si="22"/>
+        <v>16840.909090909092</v>
+      </c>
+      <c r="D216" s="1">
+        <f t="shared" si="19"/>
+        <v>17684.34247359481</v>
+      </c>
+      <c r="E216" s="1">
+        <f t="shared" si="20"/>
+        <v>6579.3687962483255</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A217" s="1">
+        <v>1800</v>
+      </c>
+      <c r="B217" s="1">
+        <f t="shared" si="21"/>
+        <v>8348.484848484848</v>
+      </c>
+      <c r="C217" s="1">
+        <f t="shared" si="22"/>
+        <v>12522.727272727272</v>
+      </c>
+      <c r="D217" s="1">
+        <f t="shared" si="19"/>
+        <v>16133.934366320744</v>
+      </c>
+      <c r="E217" s="1">
+        <f t="shared" si="20"/>
+        <v>6002.5474223306637</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A218" s="1">
+        <v>1801</v>
+      </c>
+      <c r="B218" s="1">
+        <f t="shared" si="21"/>
+        <v>5277.7777777777774</v>
+      </c>
+      <c r="C218" s="1">
+        <f t="shared" si="22"/>
+        <v>7916.6666666666661</v>
+      </c>
+      <c r="D218" s="1">
+        <f t="shared" si="19"/>
+        <v>9665.825543786752</v>
+      </c>
+      <c r="E218" s="1">
+        <f t="shared" si="20"/>
+        <v>3596.1207530179199</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A219" s="1">
+        <v>1802</v>
+      </c>
+      <c r="D219" s="1">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="E219" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A220" s="1">
+        <v>1803</v>
+      </c>
+      <c r="D220" s="1">
+        <f t="shared" si="19"/>
+        <v>5377.9781221069152</v>
+      </c>
+      <c r="E220" s="1">
+        <f t="shared" si="20"/>
+        <v>2000.8491407768881</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A221" s="1">
+        <v>1804</v>
+      </c>
+      <c r="D221" s="1">
+        <f t="shared" si="19"/>
+        <v>9375.1240236728645</v>
+      </c>
+      <c r="E221" s="1">
+        <f t="shared" si="20"/>
+        <v>3487.9667454083587</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A222" s="1">
+        <v>1805</v>
+      </c>
+      <c r="D222" s="1">
+        <f t="shared" si="19"/>
+        <v>12282.139224811737</v>
+      </c>
+      <c r="E222" s="1">
+        <f t="shared" si="20"/>
+        <v>4569.5068215039746</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A223" s="1">
+        <v>1806</v>
+      </c>
+      <c r="D223" s="1">
+        <f t="shared" si="19"/>
+        <v>12572.840744925625</v>
+      </c>
+      <c r="E223" s="1">
+        <f t="shared" si="20"/>
+        <v>4677.6608291135353</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A224" s="1">
+        <v>1807</v>
+      </c>
+      <c r="D224" s="1">
+        <f t="shared" si="19"/>
+        <v>13541.845811971916</v>
+      </c>
+      <c r="E224" s="1">
+        <f t="shared" si="20"/>
+        <v>5038.1741878120738</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225" s="1">
+        <v>1808</v>
+      </c>
+      <c r="D225" s="1">
+        <f t="shared" si="19"/>
+        <v>11361.584411117761</v>
+      </c>
+      <c r="E225" s="1">
+        <f t="shared" si="20"/>
+        <v>4227.0191307403629</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" s="1">
+        <v>1809</v>
+      </c>
+      <c r="D226" s="1">
+        <f t="shared" si="19"/>
+        <v>13832.547332085804</v>
+      </c>
+      <c r="E226" s="1">
+        <f t="shared" si="20"/>
+        <v>5146.3281954216354</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227" s="1">
+        <v>1810</v>
+      </c>
+      <c r="D227" s="1">
+        <f t="shared" si="19"/>
+        <v>14995.353412541352</v>
+      </c>
+      <c r="E227" s="1">
+        <f t="shared" si="20"/>
+        <v>5578.944225859882</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228" s="1">
+        <v>1811</v>
+      </c>
+      <c r="D228" s="1">
+        <f t="shared" si="19"/>
+        <v>11385.809537793919</v>
+      </c>
+      <c r="E228" s="1">
+        <f t="shared" si="20"/>
+        <v>4236.0319647078259</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229" s="1">
+        <v>1812</v>
+      </c>
+      <c r="D229" s="1">
+        <f t="shared" si="19"/>
+        <v>11506.935171174706</v>
+      </c>
+      <c r="E229" s="1">
+        <f t="shared" si="20"/>
+        <v>4281.0961345451433</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230" s="1">
+        <v>1813</v>
+      </c>
+      <c r="D230" s="1">
+        <f t="shared" si="19"/>
+        <v>8987.5219968543479</v>
+      </c>
+      <c r="E230" s="1">
+        <f t="shared" si="20"/>
+        <v>3343.7614019289431</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A231" s="1">
+        <v>1814</v>
+      </c>
+      <c r="D231" s="1">
+        <f t="shared" si="19"/>
+        <v>3512.6433680428045</v>
+      </c>
+      <c r="E231" s="1">
+        <f t="shared" si="20"/>
+        <v>1306.8609252822016</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F52ADF-FFA8-0A46-9CC0-C7AD4F73CE98}">
+  <dimension ref="A1:C72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1744</v>
+      </c>
+      <c r="B2" s="1">
+        <f>Calcul!B42</f>
+        <v>9360.5419791403019</v>
+      </c>
+      <c r="C2" s="1">
+        <f>Calcul!B25</f>
+        <v>5575.554826863925</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1745</v>
+      </c>
+      <c r="B3" s="1">
+        <f>Calcul!B43</f>
+        <v>16809.35865041571</v>
+      </c>
+      <c r="C3" s="1">
+        <f>Calcul!B26</f>
+        <v>10012.401094794281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1746</v>
+      </c>
+      <c r="B4" s="1">
+        <f>Calcul!B44</f>
+        <v>17059.364373168148</v>
+      </c>
+      <c r="C4" s="1">
+        <f>Calcul!B27</f>
+        <v>10161.315614631088</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1747</v>
+      </c>
+      <c r="B5" s="1">
+        <f>Calcul!B45</f>
+        <v>12445.762981954955</v>
+      </c>
+      <c r="C5" s="1">
+        <f>Calcul!B28</f>
+        <v>7413.2495770737905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1748</v>
+      </c>
+      <c r="B6" s="1">
+        <f>Calcul!B46</f>
+        <v>6473.6748871199152</v>
+      </c>
+      <c r="C6" s="1">
+        <f>Calcul!B29</f>
+        <v>3856.0084816524932</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1749</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1756</v>
+      </c>
+      <c r="B14" s="1">
+        <f>Calcul!B94+Calcul!D94</f>
+        <v>8943.4195369725203</v>
+      </c>
+      <c r="C14" s="1">
+        <f>Calcul!B68</f>
+        <v>3380.4385964912281</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1757</v>
+      </c>
+      <c r="B15" s="1">
+        <f>Calcul!B95+Calcul!D95</f>
+        <v>12192.040782193719</v>
+      </c>
+      <c r="C15" s="1">
+        <f>Calcul!B69</f>
+        <v>10628.473684210527</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1758</v>
+      </c>
+      <c r="B16" s="1">
+        <f>Calcul!B96+Calcul!D96</f>
+        <v>6793.4339992911191</v>
+      </c>
+      <c r="C16" s="1">
+        <f>Calcul!B70</f>
+        <v>5697.5614035087719</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1759</v>
+      </c>
+      <c r="B17" s="1">
+        <f>Calcul!B97+Calcul!D97</f>
+        <v>7910.4598246606784</v>
+      </c>
+      <c r="C17" s="1">
+        <f>Calcul!B71</f>
+        <v>2858.9298245614036</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1760</v>
+      </c>
+      <c r="B18" s="1">
+        <f>Calcul!B98+Calcul!D98</f>
+        <v>15976.749856030099</v>
+      </c>
+      <c r="C18" s="1">
+        <f>Calcul!B72</f>
+        <v>3438.2105263157896</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1761</v>
+      </c>
+      <c r="B19" s="1">
+        <f>Calcul!B99+Calcul!D99</f>
+        <v>7771.1921690637191</v>
+      </c>
+      <c r="C19" s="1">
+        <f>Calcul!B73</f>
+        <v>3091.5789473684208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1762</v>
+      </c>
+      <c r="B20" s="1">
+        <f>Calcul!B100+Calcul!D100</f>
+        <v>5029.703448969447</v>
+      </c>
+      <c r="C20" s="1">
+        <f>Calcul!B74</f>
+        <v>3479.5877192982457</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1763</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1778</v>
+      </c>
+      <c r="B36" s="1">
+        <f>Calcul!B130+Calcul!B156</f>
+        <v>14930.418512184069</v>
+      </c>
+      <c r="C36" s="1">
+        <f>Calcul!B138</f>
+        <v>2818.521699424497</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1779</v>
+      </c>
+      <c r="B37" s="1">
+        <f>Calcul!B131+Calcul!B157</f>
+        <v>10619.801488108289</v>
+      </c>
+      <c r="C37" s="1">
+        <f>Calcul!B139</f>
+        <v>4086.8564641655207</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1780</v>
+      </c>
+      <c r="B38" s="1">
+        <f>Calcul!B132+Calcul!B158</f>
+        <v>15067.169524477773</v>
+      </c>
+      <c r="C38" s="1">
+        <f>Calcul!B140</f>
+        <v>6482.5999086763431</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1781</v>
+      </c>
+      <c r="B39" s="1">
+        <f>Calcul!B133+Calcul!B159</f>
+        <v>19371.939364703474</v>
+      </c>
+      <c r="C39" s="1">
+        <f>Calcul!B141</f>
+        <v>6623.5259936475677</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1782</v>
+      </c>
+      <c r="B40" s="1">
+        <f>Calcul!B134+Calcul!B160</f>
+        <v>14202.005584060576</v>
+      </c>
+      <c r="C40" s="1">
+        <f>Calcul!B142</f>
+        <v>7469.0825034749168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1783</v>
+      </c>
+      <c r="B41" s="1">
+        <f>Calcul!B135+Calcul!B161</f>
+        <v>808.6655264658159</v>
+      </c>
+      <c r="C41" s="1">
+        <f>Calcul!B143</f>
+        <v>422.77825491367457</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1784</v>
+      </c>
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1793</v>
+      </c>
+      <c r="B51" s="1">
+        <f>Calcul!D210</f>
+        <v>8527.2445900073599</v>
+      </c>
+      <c r="C51" s="1">
+        <f>Calcul!E210</f>
+        <v>3172.5175565471377</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1794</v>
+      </c>
+      <c r="B52" s="1">
+        <f>Calcul!D211</f>
+        <v>15600.981579445284</v>
+      </c>
+      <c r="C52" s="1">
+        <f>Calcul!E211</f>
+        <v>5804.2650750464682</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>1795</v>
+      </c>
+      <c r="B53" s="1">
+        <f>Calcul!D212</f>
+        <v>15504.081072740655</v>
+      </c>
+      <c r="C53" s="1">
+        <f>Calcul!E212</f>
+        <v>5768.2137391766146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>1796</v>
+      </c>
+      <c r="B54" s="1">
+        <f>Calcul!D213</f>
+        <v>11846.086944640907</v>
+      </c>
+      <c r="C54" s="1">
+        <f>Calcul!E213</f>
+        <v>4407.2758100896317</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>1797</v>
+      </c>
+      <c r="B55" s="1">
+        <f>Calcul!D214</f>
+        <v>22989.645215673252</v>
+      </c>
+      <c r="C55" s="1">
+        <f>Calcul!E214</f>
+        <v>8553.1794351228236</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>1798</v>
+      </c>
+      <c r="B56" s="1">
+        <f>Calcul!D215</f>
+        <v>16666.887153196203</v>
+      </c>
+      <c r="C56" s="1">
+        <f>Calcul!E215</f>
+        <v>6200.8297696148602</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>1799</v>
+      </c>
+      <c r="B57" s="1">
+        <f>Calcul!D216</f>
+        <v>17684.34247359481</v>
+      </c>
+      <c r="C57" s="1">
+        <f>Calcul!E216</f>
+        <v>6579.3687962483255</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>1800</v>
+      </c>
+      <c r="B58" s="1">
+        <f>Calcul!D217</f>
+        <v>16133.934366320744</v>
+      </c>
+      <c r="C58" s="1">
+        <f>Calcul!E217</f>
+        <v>6002.5474223306637</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>1801</v>
+      </c>
+      <c r="B59" s="1">
+        <f>Calcul!D218</f>
+        <v>9665.825543786752</v>
+      </c>
+      <c r="C59" s="1">
+        <f>Calcul!E218</f>
+        <v>3596.1207530179199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1802</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>1803</v>
+      </c>
+      <c r="B61" s="1">
+        <f>Calcul!D220</f>
+        <v>5377.9781221069152</v>
+      </c>
+      <c r="C61" s="1">
+        <f>Calcul!E220</f>
+        <v>2000.8491407768881</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>1804</v>
+      </c>
+      <c r="B62" s="1">
+        <f>Calcul!D221</f>
+        <v>9375.1240236728645</v>
+      </c>
+      <c r="C62" s="1">
+        <f>Calcul!E221</f>
+        <v>3487.9667454083587</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>1805</v>
+      </c>
+      <c r="B63" s="1">
+        <f>Calcul!D222</f>
+        <v>12282.139224811737</v>
+      </c>
+      <c r="C63" s="1">
+        <f>Calcul!E222</f>
+        <v>4569.5068215039746</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>1806</v>
+      </c>
+      <c r="B64" s="1">
+        <f>Calcul!D223</f>
+        <v>12572.840744925625</v>
+      </c>
+      <c r="C64" s="1">
+        <f>Calcul!E223</f>
+        <v>4677.6608291135353</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>1807</v>
+      </c>
+      <c r="B65" s="1">
+        <f>Calcul!D224</f>
+        <v>13541.845811971916</v>
+      </c>
+      <c r="C65" s="1">
+        <f>Calcul!E224</f>
+        <v>5038.1741878120738</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>1808</v>
+      </c>
+      <c r="B66" s="1">
+        <f>Calcul!D225</f>
+        <v>11361.584411117761</v>
+      </c>
+      <c r="C66" s="1">
+        <f>Calcul!E225</f>
+        <v>4227.0191307403629</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>1809</v>
+      </c>
+      <c r="B67" s="1">
+        <f>Calcul!D226</f>
+        <v>13832.547332085804</v>
+      </c>
+      <c r="C67" s="1">
+        <f>Calcul!E226</f>
+        <v>5146.3281954216354</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>1810</v>
+      </c>
+      <c r="B68" s="1">
+        <f>Calcul!D227</f>
+        <v>14995.353412541352</v>
+      </c>
+      <c r="C68" s="1">
+        <f>Calcul!E227</f>
+        <v>5578.944225859882</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>1811</v>
+      </c>
+      <c r="B69" s="1">
+        <f>Calcul!D228</f>
+        <v>11385.809537793919</v>
+      </c>
+      <c r="C69" s="1">
+        <f>Calcul!E228</f>
+        <v>4236.0319647078259</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>1812</v>
+      </c>
+      <c r="B70" s="1">
+        <f>Calcul!D229</f>
+        <v>11506.935171174706</v>
+      </c>
+      <c r="C70" s="1">
+        <f>Calcul!E229</f>
+        <v>4281.0961345451433</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>1813</v>
+      </c>
+      <c r="B71" s="1">
+        <f>Calcul!D230</f>
+        <v>8987.5219968543479</v>
+      </c>
+      <c r="C71" s="1">
+        <f>Calcul!E230</f>
+        <v>3343.7614019289431</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>1814</v>
+      </c>
+      <c r="B72" s="1">
+        <f>Calcul!D231</f>
+        <v>3512.6433680428045</v>
+      </c>
+      <c r="C72" s="1">
+        <f>Calcul!E231</f>
+        <v>1306.8609252822016</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Introducing new data for French prizes 1793-1815
Signed-off-by: Guillaume Daudin <gdaudin@mac.com>
</commit_message>
<xml_diff>
--- a/External Data/Résultats de la course française.xlsx
+++ b/External Data/Résultats de la course française.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumedaudin/Répertoires Git/2016-Hamburg-Impact-of-War/External Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CB1F67-5FA0-014A-9570-AB79F1D65A4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEB8D32-25DB-F147-858E-FEF2A55369E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="-14620" windowWidth="26880" windowHeight="14620" xr2:uid="{E3D52932-A783-EC49-8617-8937D12F747E}"/>
+    <workbookView xWindow="1160" yWindow="-14620" windowWidth="26880" windowHeight="14620" activeTab="1" xr2:uid="{E3D52932-A783-EC49-8617-8937D12F747E}"/>
   </bookViews>
   <sheets>
     <sheet name="Calcul" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="226">
   <si>
     <t>Estimation de l’armement corsaire à Dunkerque, Saint-Malo et Bayonne (en milliers de lt) Villier 2002, p. 327</t>
   </si>
@@ -1069,6 +1069,12 @@
   </si>
   <si>
     <t>Valeur des prises --1797 prizes</t>
+  </si>
+  <si>
+    <t>Crowhurst via Hillmann (et UKDA)</t>
+  </si>
+  <si>
+    <t>Il y a 6 vaisseaux sans date</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1219,6 +1225,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
@@ -1554,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747C72A1-6A8D-9E42-88DE-481B3F912E70}">
-  <dimension ref="A1:O524"/>
+  <dimension ref="A1:O551"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A499" workbookViewId="0">
-      <selection activeCell="E502" sqref="E502"/>
+    <sheetView topLeftCell="A527" workbookViewId="0">
+      <selection activeCell="H539" sqref="H539"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6748,7 +6757,7 @@
         <v>1757</v>
       </c>
       <c r="B360" s="1">
-        <f t="shared" ref="B359:B365" si="34">(B346+C346+D346)*$H$356</f>
+        <f t="shared" ref="B360:B365" si="34">(B346+C346+D346)*$H$356</f>
         <v>10628.473684210527</v>
       </c>
       <c r="M360" s="1">
@@ -6857,7 +6866,7 @@
         <v>1182.06</v>
       </c>
       <c r="C370" s="1">
-        <f>(N370*I$377+M358*J$377)*$M$382</f>
+        <f t="shared" ref="C370:C376" si="35">(N370*I$377+M358*J$377)*$M$382</f>
         <v>1530.65412679474</v>
       </c>
       <c r="D370" s="1">
@@ -6891,19 +6900,19 @@
         <v>1568.0419999999999</v>
       </c>
       <c r="C371" s="1">
-        <f>(N371*I$377+M359*J$377)*$M$382</f>
+        <f t="shared" si="35"/>
         <v>2490.7132768923552</v>
       </c>
       <c r="D371" s="1">
         <v>2662.0610000000001</v>
       </c>
       <c r="E371" s="1">
-        <f t="shared" ref="E371:E377" si="35">SUM(B371:D371)</f>
+        <f t="shared" ref="E371:E377" si="36">SUM(B371:D371)</f>
         <v>6720.8162768923557</v>
       </c>
       <c r="F371" s="1"/>
       <c r="G371" s="2">
-        <f t="shared" ref="G371:G377" si="36">E371/E346</f>
+        <f t="shared" ref="G371:G377" si="37">E371/E346</f>
         <v>0.98733895649953807</v>
       </c>
       <c r="I371" s="1">
@@ -6930,18 +6939,18 @@
         <v>2450.9899999999998</v>
       </c>
       <c r="C372" s="1">
-        <f>(N372*I$377+M360*J$377)*$M$382</f>
+        <f t="shared" si="35"/>
         <v>428.5767469683355</v>
       </c>
       <c r="D372" s="1">
         <v>865.28800000000001</v>
       </c>
       <c r="E372" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>3744.8547469683353</v>
       </c>
       <c r="G372" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1.0262687714355536</v>
       </c>
       <c r="I372" s="1">
@@ -6964,18 +6973,18 @@
         <v>2626.9</v>
       </c>
       <c r="C373" s="1">
-        <f>(N373*I$377+M361*J$377)*$M$382</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="D373" s="1">
         <v>1733.711</v>
       </c>
       <c r="E373" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>4360.6109999999999</v>
       </c>
       <c r="G373" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>2.3815461496450028</v>
       </c>
       <c r="I373" s="1">
@@ -6998,18 +7007,18 @@
         <v>4335.57</v>
       </c>
       <c r="C374" s="1">
-        <f>(N374*I$377+M362*J$377)*$M$382</f>
+        <f t="shared" si="35"/>
         <v>1852.3018108969927</v>
       </c>
       <c r="D374" s="1">
         <v>2619.2510000000002</v>
       </c>
       <c r="E374" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>8807.1228108969917</v>
       </c>
       <c r="G374" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>3.9996016398260634</v>
       </c>
       <c r="I374" s="1">
@@ -7032,18 +7041,18 @@
         <v>584.55600000000004</v>
       </c>
       <c r="C375" s="1">
-        <f>(N375*I$377+M363*J$377)*$M$382</f>
+        <f t="shared" si="35"/>
         <v>641.95423263612508</v>
       </c>
       <c r="D375" s="1">
         <v>3057.33</v>
       </c>
       <c r="E375" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>4283.8402326361247</v>
       </c>
       <c r="G375" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>2.1635556730485477</v>
       </c>
       <c r="I375" s="1">
@@ -7066,18 +7075,18 @@
         <v>352.976</v>
       </c>
       <c r="C376" s="1">
-        <f>(N376*I$377+M364*J$377)*$M$382</f>
+        <f t="shared" si="35"/>
         <v>493.71096512981376</v>
       </c>
       <c r="D376" s="1">
         <v>1925.9179999999999</v>
       </c>
       <c r="E376" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>2772.6049651298135</v>
       </c>
       <c r="G376" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>1.2441574894008587</v>
       </c>
       <c r="I376" s="1">
@@ -7098,19 +7107,19 @@
         <v>13101.094000000001</v>
       </c>
       <c r="C377" s="1">
-        <f t="shared" ref="C377:D377" si="37">SUM(C370:C376)</f>
+        <f t="shared" ref="C377:D377" si="38">SUM(C370:C376)</f>
         <v>7437.9111593183625</v>
       </c>
       <c r="D377" s="1">
+        <f t="shared" si="38"/>
+        <v>15080.870999999999</v>
+      </c>
+      <c r="E377" s="1">
+        <f t="shared" si="36"/>
+        <v>35619.876159318359</v>
+      </c>
+      <c r="G377" s="2">
         <f t="shared" si="37"/>
-        <v>15080.870999999999</v>
-      </c>
-      <c r="E377" s="1">
-        <f t="shared" si="35"/>
-        <v>35619.876159318359</v>
-      </c>
-      <c r="G377" s="2">
-        <f t="shared" si="36"/>
         <v>1.7073637464023179</v>
       </c>
       <c r="I377" s="1">
@@ -7200,7 +7209,7 @@
         <v>1757</v>
       </c>
       <c r="B386" s="1">
-        <f t="shared" ref="B385:B391" si="38">B360*E371/E346</f>
+        <f t="shared" ref="B386:B391" si="39">B360*E371/E346</f>
         <v>10493.906116551223</v>
       </c>
       <c r="C386" s="2">
@@ -7208,7 +7217,7 @@
         <v>0.98733895649953818</v>
       </c>
       <c r="D386" s="1">
-        <f t="shared" ref="D386:D391" si="39">$A$395*B386/$B$392</f>
+        <f t="shared" ref="D386:D391" si="40">$A$395*B386/$B$392</f>
         <v>1698.1346656424962</v>
       </c>
     </row>
@@ -7217,15 +7226,15 @@
         <v>1758</v>
       </c>
       <c r="B387" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>5847.2293417575765</v>
       </c>
       <c r="C387" s="2">
-        <f t="shared" ref="C385:C392" si="40">B387/B361</f>
+        <f t="shared" ref="C387:C392" si="41">B387/B361</f>
         <v>1.0262687714355536</v>
       </c>
       <c r="D387" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>946.20465753354233</v>
       </c>
     </row>
@@ -7234,15 +7243,15 @@
         <v>1759</v>
       </c>
       <c r="B388" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6808.6733157894741</v>
       </c>
       <c r="C388" s="2">
+        <f t="shared" si="41"/>
+        <v>2.3815461496450028</v>
+      </c>
+      <c r="D388" s="1">
         <f t="shared" si="40"/>
-        <v>2.3815461496450028</v>
-      </c>
-      <c r="D388" s="1">
-        <f t="shared" si="39"/>
         <v>1101.7865088712038</v>
       </c>
     </row>
@@ -7251,15 +7260,15 @@
         <v>1760</v>
       </c>
       <c r="B389" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>13751.472459119865</v>
       </c>
       <c r="C389" s="2">
+        <f t="shared" si="41"/>
+        <v>3.9996016398260634</v>
+      </c>
+      <c r="D389" s="1">
         <f t="shared" si="40"/>
-        <v>3.9996016398260634</v>
-      </c>
-      <c r="D389" s="1">
-        <f t="shared" si="39"/>
         <v>2225.2773969102354</v>
       </c>
     </row>
@@ -7268,15 +7277,15 @@
         <v>1761</v>
       </c>
       <c r="B390" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6688.8031702564049</v>
       </c>
       <c r="C390" s="2">
+        <f t="shared" si="41"/>
+        <v>2.1635556730485477</v>
+      </c>
+      <c r="D390" s="1">
         <f t="shared" si="40"/>
-        <v>2.1635556730485477</v>
-      </c>
-      <c r="D390" s="1">
-        <f t="shared" si="39"/>
         <v>1082.3889988073142</v>
       </c>
     </row>
@@ -7285,15 +7294,15 @@
         <v>1762</v>
       </c>
       <c r="B391" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>4329.1551209921654</v>
       </c>
       <c r="C391" s="2">
+        <f t="shared" si="41"/>
+        <v>1.2441574894008587</v>
+      </c>
+      <c r="D391" s="1">
         <f t="shared" si="40"/>
-        <v>1.2441574894008587</v>
-      </c>
-      <c r="D391" s="1">
-        <f t="shared" si="39"/>
         <v>700.54832797728193</v>
       </c>
     </row>
@@ -7303,7 +7312,7 @@
         <v>55616.999617181304</v>
       </c>
       <c r="C392" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>1.7073637464023181</v>
       </c>
       <c r="D392" s="1">
@@ -7512,7 +7521,7 @@
         <v>1779</v>
       </c>
       <c r="B422" s="1">
-        <f t="shared" ref="B422:B426" si="41">B414/$B$419*$A$399</f>
+        <f t="shared" ref="B422:B426" si="42">B414/$B$419*$A$399</f>
         <v>5858.5858585858587</v>
       </c>
     </row>
@@ -7521,7 +7530,7 @@
         <v>1780</v>
       </c>
       <c r="B423" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>9292.9292929292933</v>
       </c>
     </row>
@@ -7530,7 +7539,7 @@
         <v>1781</v>
       </c>
       <c r="B424" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>9494.9494949494947</v>
       </c>
     </row>
@@ -7539,7 +7548,7 @@
         <v>1782</v>
       </c>
       <c r="B425" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>10707.070707070707</v>
       </c>
     </row>
@@ -7548,7 +7557,7 @@
         <v>1783</v>
       </c>
       <c r="B426" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>606.06060606060612</v>
       </c>
     </row>
@@ -7577,7 +7586,7 @@
         <v>1779</v>
       </c>
       <c r="B430" s="1">
-        <f t="shared" ref="B430:B434" si="42">B414/$B$419*$B$410</f>
+        <f t="shared" ref="B430:B434" si="43">B414/$B$419*$B$410</f>
         <v>4086.8564641655207</v>
       </c>
     </row>
@@ -7586,7 +7595,7 @@
         <v>1780</v>
       </c>
       <c r="B431" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>6482.5999086763431</v>
       </c>
       <c r="C431" s="1"/>
@@ -7608,7 +7617,7 @@
         <v>1781</v>
       </c>
       <c r="B432" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>6623.5259936475677</v>
       </c>
     </row>
@@ -7617,7 +7626,7 @@
         <v>1782</v>
       </c>
       <c r="B433" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>7469.0825034749168</v>
       </c>
     </row>
@@ -7626,7 +7635,7 @@
         <v>1783</v>
       </c>
       <c r="B434" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>422.77825491367457</v>
       </c>
     </row>
@@ -7714,7 +7723,7 @@
         <v>1779</v>
       </c>
       <c r="B448" s="1">
-        <f t="shared" ref="B448:B452" si="43">$A$401/$B$444*B439</f>
+        <f t="shared" ref="B448:B452" si="44">$A$401/$B$444*B439</f>
         <v>4761.2156295224313</v>
       </c>
     </row>
@@ -7723,7 +7732,7 @@
         <v>1780</v>
       </c>
       <c r="B449" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>5774.2402315484806</v>
       </c>
     </row>
@@ -7732,7 +7741,7 @@
         <v>1781</v>
       </c>
       <c r="B450" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>9876.9898697539793</v>
       </c>
     </row>
@@ -7741,7 +7750,7 @@
         <v>1782</v>
       </c>
       <c r="B451" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>3494.9348769898697</v>
       </c>
     </row>
@@ -7750,7 +7759,7 @@
         <v>1783</v>
       </c>
       <c r="B452" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>202.60492040520984</v>
       </c>
       <c r="D452" s="1" t="s">
@@ -8083,1010 +8092,1273 @@
         <v>55</v>
       </c>
     </row>
-    <row r="498" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A498" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C498" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A499" s="15">
+        <v>1793</v>
+      </c>
+      <c r="B499">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A500" s="15">
+        <v>1794</v>
+      </c>
+      <c r="B500">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A501" s="15">
+        <v>1795</v>
+      </c>
+      <c r="B501">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A502" s="15">
+        <v>1796</v>
+      </c>
+      <c r="B502">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A503" s="15">
+        <v>1797</v>
+      </c>
+      <c r="B503">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A504" s="15">
+        <v>1798</v>
+      </c>
+      <c r="B504">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A505" s="15">
+        <v>1799</v>
+      </c>
+      <c r="B505">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A506" s="15">
+        <v>1800</v>
+      </c>
+      <c r="B506">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A507" s="15">
+        <v>1801</v>
+      </c>
+      <c r="B507">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A508" s="15">
+        <v>1802</v>
+      </c>
+      <c r="B508">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A509" s="15">
+        <v>1803</v>
+      </c>
+      <c r="B509">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A510" s="15">
+        <v>1804</v>
+      </c>
+      <c r="B510">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A511" s="15">
+        <v>1805</v>
+      </c>
+      <c r="B511">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A512" s="15">
+        <v>1806</v>
+      </c>
+      <c r="B512">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="513" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A513" s="15">
+        <v>1807</v>
+      </c>
+      <c r="B513">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="514" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A514" s="15">
+        <v>1808</v>
+      </c>
+      <c r="B514">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="515" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A515" s="15">
+        <v>1809</v>
+      </c>
+      <c r="B515">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="516" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A516" s="15">
+        <v>1810</v>
+      </c>
+      <c r="B516">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="517" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A517" s="15">
+        <v>1811</v>
+      </c>
+      <c r="B517">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="518" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A518" s="15">
+        <v>1812</v>
+      </c>
+      <c r="B518">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="519" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A519" s="15">
+        <v>1813</v>
+      </c>
+      <c r="B519">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="520" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A520" s="15">
+        <v>1814</v>
+      </c>
+      <c r="B520">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="521" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A521" s="15">
+        <v>1815</v>
+      </c>
+      <c r="B521">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="522" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A522" s="15"/>
+      <c r="B522"/>
+    </row>
+    <row r="523" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A523" s="15"/>
+      <c r="B523"/>
+    </row>
+    <row r="524" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A524" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="499" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A499" s="1" t="s">
+    <row r="525" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A525" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D499" s="1">
+      <c r="D525" s="1">
         <f>19000/198</f>
         <v>95.959595959595958</v>
       </c>
-      <c r="F499" s="1" t="s">
+      <c r="F525" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="J499" s="1">
-        <f>AVERAGE(F503,F506:F511)</f>
-        <v>32.56164157679305</v>
-      </c>
-    </row>
-    <row r="501" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C501" s="1" t="s">
+      <c r="J525" s="1">
+        <f>AVERAGE(F529,F532:F537)</f>
+        <v>58.929551037162881</v>
+      </c>
+    </row>
+    <row r="527" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C527" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="L501" s="12" t="s">
+      <c r="L527" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="O501" s="2">
+      <c r="O527" s="2">
         <f>B395/(1+B395)</f>
         <v>0.13928223305507595</v>
       </c>
     </row>
-    <row r="502" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B502" s="1" t="s">
+    <row r="528" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B528" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C502" s="1" t="s">
+      <c r="C528" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D502" s="1" t="s">
+      <c r="D528" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E502" s="1" t="s">
+      <c r="E528" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="F502" s="1" t="s">
+      <c r="F528" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="H502" s="1" t="s">
+      <c r="H528" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="K502" s="1">
+      <c r="K528" s="1">
         <v>1789</v>
       </c>
-      <c r="L502" s="12">
+      <c r="L528" s="12">
         <v>4.4539999999999997</v>
       </c>
-      <c r="M502" s="1" t="s">
+      <c r="M528" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="O502" s="1" t="s">
+      <c r="O528" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="503" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A503" s="1">
+    <row r="529" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A529" s="1">
         <v>1793</v>
       </c>
-      <c r="B503" s="1">
-        <f>B488*$D$499*$L$502/L503*M503</f>
-        <v>37993.010631143021</v>
-      </c>
-      <c r="C503" s="1">
-        <f>B503*$C$410</f>
-        <v>54463.697651335431</v>
-      </c>
-      <c r="D503" s="1">
-        <f>C503*0.15</f>
-        <v>8169.5546477003145</v>
-      </c>
-      <c r="E503" s="1">
-        <f>(C503+D503)/B462</f>
-        <v>177.93537584953336</v>
-      </c>
-      <c r="F503" s="1">
-        <f>E503*L503/$L$507*M503/M$507</f>
-        <v>64.217145319436227</v>
-      </c>
-      <c r="H503" s="1">
-        <f>C503+D503</f>
-        <v>62633.252299035747</v>
-      </c>
-      <c r="K503" s="1">
+      <c r="B529" s="1">
+        <f>B499*$D$525*$L$528/L529*M529</f>
+        <v>52384.302536878997</v>
+      </c>
+      <c r="C529" s="1">
+        <f>B529*$C$410</f>
+        <v>75093.886155629138</v>
+      </c>
+      <c r="D529" s="1">
+        <f>C529*0.15</f>
+        <v>11264.082923344371</v>
+      </c>
+      <c r="E529" s="1">
+        <f>(C529+D529)/B462</f>
+        <v>245.33513942890201</v>
+      </c>
+      <c r="F529" s="1">
+        <f>E529*L529/$L$533*M529/M$533</f>
+        <v>88.541821576798412</v>
+      </c>
+      <c r="H529" s="1">
+        <f>C529+D529</f>
+        <v>86357.969078973503</v>
+      </c>
+      <c r="K529" s="1">
         <v>1793</v>
       </c>
-      <c r="L503" s="12">
+      <c r="L529" s="12">
         <v>1.69</v>
       </c>
-      <c r="M503" s="2">
-        <f>(1+0.01)^N503</f>
+      <c r="M529" s="2">
+        <f>(1+0.01)^N529</f>
         <v>1.1380932804332895</v>
       </c>
-      <c r="N503" s="1">
+      <c r="N529" s="1">
         <v>13</v>
       </c>
-      <c r="O503" s="1">
-        <f>E503</f>
-        <v>177.93537584953336</v>
-      </c>
-    </row>
-    <row r="504" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A504" s="1">
+      <c r="O529" s="1">
+        <f>E529</f>
+        <v>245.33513942890201</v>
+      </c>
+    </row>
+    <row r="530" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A530" s="1">
         <v>1794</v>
       </c>
-      <c r="C504" s="1">
+      <c r="B530" s="1">
+        <f t="shared" ref="B530:B551" si="45">B500*$D$525*$L$528/L530*M530</f>
+        <v>2748.4750941427433</v>
+      </c>
+      <c r="C530" s="1">
+        <f t="shared" ref="C530:C551" si="46">B530*$C$410</f>
+        <v>3939.99090998366</v>
+      </c>
+      <c r="D530" s="1">
+        <f t="shared" ref="D530:D551" si="47">C530*0.15</f>
+        <v>590.998636497549</v>
+      </c>
+      <c r="E530" s="1">
+        <f t="shared" ref="E530:E551" si="48">(C530+D530)/B463</f>
+        <v>7.0356980535422498</v>
+      </c>
+      <c r="F530" s="1">
+        <f t="shared" ref="F530:F550" si="49">E530*L530/$L$533*M530/M$533</f>
+        <v>2.1700342837385316</v>
+      </c>
+      <c r="H530" s="1">
+        <f t="shared" ref="H530:H550" si="50">C530+D530</f>
+        <v>4530.9895464812089</v>
+      </c>
+      <c r="K530" s="1">
+        <v>1794</v>
+      </c>
+      <c r="L530" s="12">
+        <v>1.43</v>
+      </c>
+      <c r="M530" s="2">
+        <f t="shared" ref="M530:M551" si="51">(1+0.01)^N530</f>
+        <v>1.1494742132376226</v>
+      </c>
+      <c r="N530" s="1">
+        <v>14</v>
+      </c>
+      <c r="O530" s="1">
+        <f t="shared" ref="O530:O550" si="52">$E$529*L$529/L530*M530/M$529</f>
+        <v>292.84094370013491</v>
+      </c>
+    </row>
+    <row r="531" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A531" s="1">
+        <v>1795</v>
+      </c>
+      <c r="B531" s="1">
+        <f t="shared" si="45"/>
+        <v>63403.693961679419</v>
+      </c>
+      <c r="C531" s="1">
+        <f t="shared" si="46"/>
+        <v>90890.391694205682</v>
+      </c>
+      <c r="D531" s="1">
+        <f t="shared" si="47"/>
+        <v>13633.558754130852</v>
+      </c>
+      <c r="E531" s="1">
+        <f t="shared" si="48"/>
+        <v>163.31867257552582</v>
+      </c>
+      <c r="F531" s="1">
+        <f t="shared" si="49"/>
+        <v>6.4040259808068134</v>
+      </c>
+      <c r="H531" s="1">
+        <f t="shared" si="50"/>
+        <v>104523.95044833653</v>
+      </c>
+      <c r="K531" s="1">
+        <v>1795</v>
+      </c>
+      <c r="L531" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="M531" s="2">
+        <f t="shared" si="51"/>
+        <v>1.1609689553699984</v>
+      </c>
+      <c r="N531" s="1">
+        <v>15</v>
+      </c>
+      <c r="O531" s="1">
+        <f t="shared" si="52"/>
+        <v>2349.7231943672487</v>
+      </c>
+    </row>
+    <row r="532" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A532" s="1">
+        <v>1796</v>
+      </c>
+      <c r="B532" s="1">
+        <f t="shared" si="45"/>
+        <v>164131.4885491918</v>
+      </c>
+      <c r="C532" s="1">
+        <f t="shared" si="46"/>
+        <v>235285.58592509385</v>
+      </c>
+      <c r="D532" s="1">
+        <f t="shared" si="47"/>
+        <v>35292.837888764079</v>
+      </c>
+      <c r="E532" s="1">
+        <f t="shared" si="48"/>
+        <v>553.33011004878927</v>
+      </c>
+      <c r="F532" s="1">
+        <f t="shared" si="49"/>
+        <v>48.697919476241076</v>
+      </c>
+      <c r="H532" s="1">
+        <f t="shared" si="50"/>
+        <v>270578.42381385795</v>
+      </c>
+      <c r="K532" s="1">
+        <v>1796</v>
+      </c>
+      <c r="L532" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="M532" s="2">
+        <f t="shared" si="51"/>
+        <v>1.1725786449236988</v>
+      </c>
+      <c r="N532" s="1">
+        <v>16</v>
+      </c>
+      <c r="O532" s="1">
+        <f t="shared" si="52"/>
+        <v>1067.9491918399146</v>
+      </c>
+    </row>
+    <row r="533" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A533" s="1">
+        <v>1797</v>
+      </c>
+      <c r="B533" s="1">
+        <f t="shared" si="45"/>
+        <v>35094.903933246031</v>
+      </c>
+      <c r="C533" s="1">
+        <f t="shared" si="46"/>
+        <v>50309.207013886757</v>
+      </c>
+      <c r="D533" s="1">
+        <f t="shared" si="47"/>
+        <v>7546.3810520830129</v>
+      </c>
+      <c r="E533" s="1">
+        <f t="shared" si="48"/>
+        <v>60.964792482581423</v>
+      </c>
+      <c r="F533" s="1">
+        <f t="shared" si="49"/>
+        <v>60.96479248258143</v>
+      </c>
+      <c r="H533" s="1">
+        <f t="shared" si="50"/>
+        <v>57855.588065969772</v>
+      </c>
+      <c r="K533" s="1">
+        <v>1797</v>
+      </c>
+      <c r="L533" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M533" s="2">
+        <f t="shared" si="51"/>
+        <v>1.1843044313729358</v>
+      </c>
+      <c r="N533" s="1">
+        <v>17</v>
+      </c>
+      <c r="O533" s="1">
+        <f t="shared" si="52"/>
+        <v>95.878105222961238</v>
+      </c>
+    </row>
+    <row r="534" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A534" s="1">
+        <v>1798</v>
+      </c>
+      <c r="B534" s="1">
+        <f t="shared" si="45"/>
+        <v>31355.946860357893</v>
+      </c>
+      <c r="C534" s="1">
+        <f t="shared" si="46"/>
+        <v>44949.34149740728</v>
+      </c>
+      <c r="D534" s="1">
+        <f t="shared" si="47"/>
+        <v>6742.4012246110915</v>
+      </c>
+      <c r="E534" s="1">
+        <f t="shared" si="48"/>
+        <v>75.133346979677867</v>
+      </c>
+      <c r="F534" s="1">
+        <f t="shared" si="49"/>
+        <v>75.884680449474658</v>
+      </c>
+      <c r="H534" s="1">
+        <f t="shared" si="50"/>
+        <v>51691.742722018374</v>
+      </c>
+      <c r="K534" s="1">
+        <v>1798</v>
+      </c>
+      <c r="L534" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M534" s="2">
+        <f t="shared" si="51"/>
+        <v>1.1961474756866652</v>
+      </c>
+      <c r="N534" s="1">
+        <v>18</v>
+      </c>
+      <c r="O534" s="1">
+        <f t="shared" si="52"/>
+        <v>96.836886275190849</v>
+      </c>
+    </row>
+    <row r="535" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A535" s="1">
+        <v>1799</v>
+      </c>
+      <c r="B535" s="1">
+        <f t="shared" si="45"/>
+        <v>22604.683865236984</v>
+      </c>
+      <c r="C535" s="1">
+        <f t="shared" si="46"/>
+        <v>32404.240861373633</v>
+      </c>
+      <c r="D535" s="1">
+        <f t="shared" si="47"/>
+        <v>4860.6361292060446</v>
+      </c>
+      <c r="E535" s="1">
+        <f t="shared" si="48"/>
+        <v>51.047776699424219</v>
+      </c>
+      <c r="F535" s="1">
+        <f t="shared" si="49"/>
+        <v>52.073837011082631</v>
+      </c>
+      <c r="H535" s="1">
+        <f t="shared" si="50"/>
+        <v>37264.87699057968</v>
+      </c>
+      <c r="K535" s="1">
+        <v>1799</v>
+      </c>
+      <c r="L535" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M535" s="2">
+        <f t="shared" si="51"/>
+        <v>1.2081089504435316</v>
+      </c>
+      <c r="N535" s="1">
+        <v>19</v>
+      </c>
+      <c r="O535" s="1">
+        <f t="shared" si="52"/>
+        <v>97.805255137942737</v>
+      </c>
+    </row>
+    <row r="536" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A536" s="1">
+        <v>1800</v>
+      </c>
+      <c r="B536" s="1">
+        <f t="shared" si="45"/>
+        <v>16688.452900304914</v>
+      </c>
+      <c r="C536" s="1">
+        <f t="shared" si="46"/>
+        <v>23923.212136437476</v>
+      </c>
+      <c r="D536" s="1">
+        <f t="shared" si="47"/>
+        <v>3588.4818204656212</v>
+      </c>
+      <c r="E536" s="1">
+        <f t="shared" si="48"/>
+        <v>41.308849785139785</v>
+      </c>
+      <c r="F536" s="1">
+        <f t="shared" si="49"/>
+        <v>42.560549242479304</v>
+      </c>
+      <c r="H536" s="1">
+        <f t="shared" si="50"/>
+        <v>27511.693956903098</v>
+      </c>
+      <c r="K536" s="1">
+        <v>1800</v>
+      </c>
+      <c r="L536" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M536" s="2">
+        <f t="shared" si="51"/>
+        <v>1.220190039947967</v>
+      </c>
+      <c r="N536" s="1">
+        <v>20</v>
+      </c>
+      <c r="O536" s="1">
+        <f t="shared" si="52"/>
+        <v>98.783307689322172</v>
+      </c>
+    </row>
+    <row r="537" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A537" s="1">
+        <v>1801</v>
+      </c>
+      <c r="B537" s="1">
+        <f t="shared" si="45"/>
+        <v>10183.433030206892</v>
+      </c>
+      <c r="C537" s="1">
+        <f t="shared" si="46"/>
+        <v>14598.143405755281</v>
+      </c>
+      <c r="D537" s="1">
+        <f t="shared" si="47"/>
+        <v>2189.7215108632922</v>
+      </c>
+      <c r="E537" s="1">
+        <f t="shared" si="48"/>
+        <v>42.074849415084145</v>
+      </c>
+      <c r="F537" s="1">
+        <f t="shared" si="49"/>
+        <v>43.783257021482704</v>
+      </c>
+      <c r="H537" s="1">
+        <f t="shared" si="50"/>
+        <v>16787.864916618575</v>
+      </c>
+      <c r="K537" s="1">
+        <v>1801</v>
+      </c>
+      <c r="L537" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M537" s="2">
+        <f t="shared" si="51"/>
+        <v>1.2323919403474466</v>
+      </c>
+      <c r="N537" s="1">
+        <v>21</v>
+      </c>
+      <c r="O537" s="1">
+        <f t="shared" si="52"/>
+        <v>99.771140766215396</v>
+      </c>
+    </row>
+    <row r="538" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A538" s="1">
+        <v>1802</v>
+      </c>
+      <c r="B538" s="1">
+        <f t="shared" si="45"/>
+        <v>472.88585565558458</v>
+      </c>
+      <c r="C538" s="1">
+        <f t="shared" si="46"/>
+        <v>677.89079723277416</v>
+      </c>
+      <c r="D538" s="1">
+        <f t="shared" si="47"/>
+        <v>101.68361958491612</v>
+      </c>
+      <c r="H538" s="1">
         <v>0</v>
       </c>
-      <c r="D504" s="3">
-        <f>B463*E504</f>
-        <v>64047.84382926664</v>
-      </c>
-      <c r="E504" s="1">
-        <f>$J$499*L$507/L504*M504/M$507</f>
-        <v>99.45317364792956</v>
-      </c>
-      <c r="H504" s="1">
-        <f>C504+D504</f>
-        <v>64047.84382926664</v>
-      </c>
-      <c r="K504" s="1">
-        <v>1794</v>
-      </c>
-      <c r="L504" s="12">
-        <v>1.43</v>
-      </c>
-      <c r="M504" s="2">
-        <f t="shared" ref="M504:M524" si="44">(1+0.01)^N504</f>
-        <v>1.1494742132376226</v>
-      </c>
-      <c r="N504" s="1">
-        <v>14</v>
-      </c>
-      <c r="O504" s="1">
-        <f>$E$503*L$503/L504*M504/M$503</f>
-        <v>212.39013499130667</v>
-      </c>
-    </row>
-    <row r="505" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A505" s="1">
-        <v>1795</v>
-      </c>
-      <c r="C505" s="1">
+      <c r="K538" s="1">
+        <v>1802</v>
+      </c>
+      <c r="L538" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M538" s="2">
+        <f t="shared" si="51"/>
+        <v>1.2447158597509214</v>
+      </c>
+      <c r="N538" s="1">
+        <v>22</v>
+      </c>
+      <c r="O538" s="1">
+        <f t="shared" si="52"/>
+        <v>100.76885217387756</v>
+      </c>
+    </row>
+    <row r="539" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A539" s="1">
+        <v>1803</v>
+      </c>
+      <c r="B539" s="1">
+        <f t="shared" si="45"/>
+        <v>9194.0832485837018</v>
+      </c>
+      <c r="C539" s="1">
+        <f t="shared" si="46"/>
+        <v>13179.89182519821</v>
+      </c>
+      <c r="D539" s="1">
+        <f t="shared" si="47"/>
+        <v>1976.9837737797316</v>
+      </c>
+      <c r="E539" s="1">
+        <f t="shared" si="48"/>
+        <v>68.274214409810554</v>
+      </c>
+      <c r="F539" s="1">
+        <f t="shared" si="49"/>
+        <v>72.474454362467057</v>
+      </c>
+      <c r="H539" s="1">
+        <f t="shared" si="50"/>
+        <v>15156.875598977942</v>
+      </c>
+      <c r="K539" s="1">
+        <v>1803</v>
+      </c>
+      <c r="L539" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M539" s="2">
+        <f t="shared" si="51"/>
+        <v>1.2571630183484304</v>
+      </c>
+      <c r="N539" s="1">
+        <v>23</v>
+      </c>
+      <c r="O539" s="1">
+        <f t="shared" si="52"/>
+        <v>101.77654069561632</v>
+      </c>
+    </row>
+    <row r="540" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A540" s="1">
+        <v>1804</v>
+      </c>
+      <c r="B540" s="1">
+        <f t="shared" si="45"/>
+        <v>4341.517752188357</v>
+      </c>
+      <c r="C540" s="1">
+        <f t="shared" si="46"/>
+        <v>6223.6476203143775</v>
+      </c>
+      <c r="D540" s="1">
+        <f t="shared" si="47"/>
+        <v>933.54714304715662</v>
+      </c>
+      <c r="E540" s="1">
+        <f t="shared" si="48"/>
+        <v>18.494043316179678</v>
+      </c>
+      <c r="F540" s="1">
+        <f t="shared" si="49"/>
+        <v>19.828117642674595</v>
+      </c>
+      <c r="H540" s="1">
+        <f t="shared" si="50"/>
+        <v>7157.1947633615346</v>
+      </c>
+      <c r="L540" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M540" s="2">
+        <f t="shared" si="51"/>
+        <v>1.269734648531915</v>
+      </c>
+      <c r="N540" s="1">
+        <v>24</v>
+      </c>
+      <c r="O540" s="1">
+        <f t="shared" si="52"/>
+        <v>102.79430610257251</v>
+      </c>
+    </row>
+    <row r="541" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A541" s="1">
+        <v>1805</v>
+      </c>
+      <c r="B541" s="1">
+        <f t="shared" si="45"/>
+        <v>3654.1107747585343</v>
+      </c>
+      <c r="C541" s="1">
+        <f t="shared" si="46"/>
+        <v>5238.2367470979352</v>
+      </c>
+      <c r="D541" s="1">
+        <f t="shared" si="47"/>
+        <v>785.73551206469028</v>
+      </c>
+      <c r="E541" s="1">
+        <f t="shared" si="48"/>
+        <v>11.881602089078156</v>
+      </c>
+      <c r="F541" s="1">
+        <f t="shared" si="49"/>
+        <v>12.866072495762889</v>
+      </c>
+      <c r="H541" s="1">
+        <f t="shared" si="50"/>
+        <v>6023.9722591626251</v>
+      </c>
+      <c r="L541" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M541" s="2">
+        <f t="shared" si="51"/>
+        <v>1.2824319950172343</v>
+      </c>
+      <c r="N541" s="1">
+        <v>25</v>
+      </c>
+      <c r="O541" s="1">
+        <f t="shared" si="52"/>
+        <v>103.82224916359824</v>
+      </c>
+    </row>
+    <row r="542" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A542" s="1">
+        <v>1806</v>
+      </c>
+      <c r="B542" s="1">
+        <f t="shared" si="45"/>
+        <v>7258.2820355953681</v>
+      </c>
+      <c r="C542" s="1">
+        <f t="shared" si="46"/>
+        <v>10404.884258652197</v>
+      </c>
+      <c r="D542" s="1">
+        <f t="shared" si="47"/>
+        <v>1560.7326387978294</v>
+      </c>
+      <c r="E542" s="1">
+        <f t="shared" si="48"/>
+        <v>23.055138530732229</v>
+      </c>
+      <c r="F542" s="1">
+        <f t="shared" si="49"/>
+        <v>25.215065470759598</v>
+      </c>
+      <c r="H542" s="1">
+        <f t="shared" si="50"/>
+        <v>11965.616897450027</v>
+      </c>
+      <c r="L542" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M542" s="2">
+        <f t="shared" si="51"/>
+        <v>1.2952563149674066</v>
+      </c>
+      <c r="N542" s="1">
+        <v>26</v>
+      </c>
+      <c r="O542" s="1">
+        <f t="shared" si="52"/>
+        <v>104.86047165523422</v>
+      </c>
+    </row>
+    <row r="543" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A543" s="1">
+        <v>1807</v>
+      </c>
+      <c r="B543" s="1">
+        <f t="shared" si="45"/>
+        <v>11928.186884259772</v>
+      </c>
+      <c r="C543" s="1">
+        <f t="shared" si="46"/>
+        <v>17099.280978286723</v>
+      </c>
+      <c r="D543" s="1">
+        <f t="shared" si="47"/>
+        <v>2564.8921467430082</v>
+      </c>
+      <c r="E543" s="1">
+        <f t="shared" si="48"/>
+        <v>35.177411672682879</v>
+      </c>
+      <c r="F543" s="1">
+        <f t="shared" si="49"/>
+        <v>38.85774724834387</v>
+      </c>
+      <c r="H543" s="1">
+        <f t="shared" si="50"/>
+        <v>19664.173125029731</v>
+      </c>
+      <c r="L543" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M543" s="2">
+        <f t="shared" si="51"/>
+        <v>1.3082088781170802</v>
+      </c>
+      <c r="N543" s="1">
+        <v>27</v>
+      </c>
+      <c r="O543" s="1">
+        <f t="shared" si="52"/>
+        <v>105.90907637178653</v>
+      </c>
+    </row>
+    <row r="544" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A544" s="1">
+        <v>1808</v>
+      </c>
+      <c r="B544" s="1">
+        <f t="shared" si="45"/>
+        <v>19075.158859078758</v>
+      </c>
+      <c r="C544" s="1">
+        <f t="shared" si="46"/>
+        <v>27344.600164443524</v>
+      </c>
+      <c r="D544" s="1">
+        <f t="shared" si="47"/>
+        <v>4101.6900246665282</v>
+      </c>
+      <c r="E544" s="1">
+        <f t="shared" si="48"/>
+        <v>67.049659251833802</v>
+      </c>
+      <c r="F544" s="1">
+        <f t="shared" si="49"/>
+        <v>74.80518248196627</v>
+      </c>
+      <c r="H544" s="1">
+        <f t="shared" si="50"/>
+        <v>31446.290189110052</v>
+      </c>
+      <c r="L544" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M544" s="2">
+        <f t="shared" si="51"/>
+        <v>1.3212909668982511</v>
+      </c>
+      <c r="N544" s="1">
+        <v>28</v>
+      </c>
+      <c r="O544" s="1">
+        <f t="shared" si="52"/>
+        <v>106.9681671355044</v>
+      </c>
+    </row>
+    <row r="545" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A545" s="1">
+        <v>1809</v>
+      </c>
+      <c r="B545" s="1">
+        <f t="shared" si="45"/>
+        <v>21293.901021108442</v>
+      </c>
+      <c r="C545" s="1">
+        <f t="shared" si="46"/>
+        <v>30525.208920413002</v>
+      </c>
+      <c r="D545" s="1">
+        <f t="shared" si="47"/>
+        <v>4578.78133806195</v>
+      </c>
+      <c r="E545" s="1">
+        <f t="shared" si="48"/>
+        <v>61.478091520971894</v>
+      </c>
+      <c r="F545" s="1">
+        <f t="shared" si="49"/>
+        <v>69.275052330575136</v>
+      </c>
+      <c r="H545" s="1">
+        <f t="shared" si="50"/>
+        <v>35103.990258474951</v>
+      </c>
+      <c r="L545" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M545" s="2">
+        <f t="shared" si="51"/>
+        <v>1.3345038765672337</v>
+      </c>
+      <c r="N545" s="1">
+        <v>29</v>
+      </c>
+      <c r="O545" s="1">
+        <f t="shared" si="52"/>
+        <v>108.03784880685946</v>
+      </c>
+    </row>
+    <row r="546" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A546" s="1">
+        <v>1810</v>
+      </c>
+      <c r="B546" s="1">
+        <f t="shared" si="45"/>
+        <v>26883.550039149417</v>
+      </c>
+      <c r="C546" s="1">
+        <f t="shared" si="46"/>
+        <v>38538.07626202143</v>
+      </c>
+      <c r="D546" s="1">
+        <f t="shared" si="47"/>
+        <v>5780.7114393032143</v>
+      </c>
+      <c r="E546" s="1">
+        <f t="shared" si="48"/>
+        <v>71.597395317164214</v>
+      </c>
+      <c r="F546" s="1">
+        <f t="shared" si="49"/>
+        <v>81.484514506990465</v>
+      </c>
+      <c r="H546" s="1">
+        <f t="shared" si="50"/>
+        <v>44318.787701324647</v>
+      </c>
+      <c r="L546" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M546" s="2">
+        <f t="shared" si="51"/>
+        <v>1.3478489153329063</v>
+      </c>
+      <c r="N546" s="1">
+        <v>30</v>
+      </c>
+      <c r="O546" s="1">
+        <f t="shared" si="52"/>
+        <v>109.11822729492808</v>
+      </c>
+    </row>
+    <row r="547" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A547" s="1">
+        <v>1811</v>
+      </c>
+      <c r="B547" s="1">
+        <f t="shared" si="45"/>
+        <v>27928.167983527783</v>
+      </c>
+      <c r="C547" s="1">
+        <f t="shared" si="46"/>
+        <v>40035.555796774242</v>
+      </c>
+      <c r="D547" s="1">
+        <f t="shared" si="47"/>
+        <v>6005.3333695161364</v>
+      </c>
+      <c r="E547" s="1">
+        <f t="shared" si="48"/>
+        <v>97.959338651681648</v>
+      </c>
+      <c r="F547" s="1">
+        <f t="shared" si="49"/>
+        <v>112.60173372591954</v>
+      </c>
+      <c r="H547" s="1">
+        <f t="shared" si="50"/>
+        <v>46040.889166290377</v>
+      </c>
+      <c r="L547" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M547" s="2">
+        <f t="shared" si="51"/>
+        <v>1.3613274044862349</v>
+      </c>
+      <c r="N547" s="1">
+        <v>31</v>
+      </c>
+      <c r="O547" s="1">
+        <f t="shared" si="52"/>
+        <v>110.20940956787732</v>
+      </c>
+    </row>
+    <row r="548" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A548" s="1">
+        <v>1812</v>
+      </c>
+      <c r="B548" s="1">
+        <f t="shared" si="45"/>
+        <v>10969.563757974527</v>
+      </c>
+      <c r="C548" s="1">
+        <f t="shared" si="46"/>
+        <v>15725.076637955222</v>
+      </c>
+      <c r="D548" s="1">
+        <f t="shared" si="47"/>
+        <v>2358.7614956932835</v>
+      </c>
+      <c r="E548" s="1">
+        <f t="shared" si="48"/>
+        <v>38.071238176102121</v>
+      </c>
+      <c r="F548" s="1">
+        <f t="shared" si="49"/>
+        <v>44.199525614951696</v>
+      </c>
+      <c r="H548" s="1">
+        <f t="shared" si="50"/>
+        <v>18083.838133648507</v>
+      </c>
+      <c r="L548" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M548" s="2">
+        <f t="shared" si="51"/>
+        <v>1.3749406785310976</v>
+      </c>
+      <c r="N548" s="1">
+        <v>32</v>
+      </c>
+      <c r="O548" s="1">
+        <f t="shared" si="52"/>
+        <v>111.31150366355611</v>
+      </c>
+    </row>
+    <row r="549" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A549" s="1">
+        <v>1813</v>
+      </c>
+      <c r="B549" s="1">
+        <f t="shared" si="45"/>
+        <v>10155.987779258083</v>
+      </c>
+      <c r="C549" s="1">
+        <f t="shared" si="46"/>
+        <v>14558.80012064021</v>
+      </c>
+      <c r="D549" s="1">
+        <f t="shared" si="47"/>
+        <v>2183.8200180960312</v>
+      </c>
+      <c r="E549" s="1">
+        <f t="shared" si="48"/>
+        <v>45.128356169100378</v>
+      </c>
+      <c r="F549" s="1">
+        <f t="shared" si="49"/>
+        <v>52.916546724397762</v>
+      </c>
+      <c r="H549" s="1">
+        <f t="shared" si="50"/>
+        <v>16742.620138736242</v>
+      </c>
+      <c r="L549" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M549" s="2">
+        <f t="shared" si="51"/>
+        <v>1.3886900853164086</v>
+      </c>
+      <c r="N549" s="1">
+        <v>33</v>
+      </c>
+      <c r="O549" s="1">
+        <f t="shared" si="52"/>
+        <v>112.42461870019169</v>
+      </c>
+    </row>
+    <row r="550" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A550" s="1">
+        <v>1814</v>
+      </c>
+      <c r="B550" s="1">
+        <f t="shared" si="45"/>
+        <v>3330.3726159255402</v>
+      </c>
+      <c r="C550" s="1">
+        <f t="shared" si="46"/>
+        <v>4774.1519876125367</v>
+      </c>
+      <c r="D550" s="1">
+        <f t="shared" si="47"/>
+        <v>716.12279814188048</v>
+      </c>
+      <c r="E550" s="1">
+        <f t="shared" si="48"/>
+        <v>37.863964039685634</v>
+      </c>
+      <c r="F550" s="1">
+        <f t="shared" si="49"/>
+        <v>44.842460401545182</v>
+      </c>
+      <c r="H550" s="1">
+        <f t="shared" si="50"/>
+        <v>5490.2747857544173</v>
+      </c>
+      <c r="L550" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="M550" s="2">
+        <f t="shared" si="51"/>
+        <v>1.4025769861695727</v>
+      </c>
+      <c r="N550" s="1">
+        <v>34</v>
+      </c>
+      <c r="O550" s="1">
+        <f>$E$529*L$529/L550*M550/M$529</f>
+        <v>113.5488648871936</v>
+      </c>
+    </row>
+    <row r="551" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A551" s="1">
+        <v>1815</v>
+      </c>
+      <c r="B551" s="1">
+        <f>B521*$D$525*$L$528/L551*M551</f>
+        <v>134.54705368339179</v>
+      </c>
+      <c r="C551" s="1">
+        <f t="shared" si="46"/>
+        <v>192.87574029954644</v>
+      </c>
+      <c r="D551" s="1">
+        <f t="shared" si="47"/>
+        <v>28.931361044931965</v>
+      </c>
+      <c r="H551" s="1">
         <v>0</v>
       </c>
-      <c r="D505" s="3">
-        <f>B464*E505</f>
-        <v>510720.77759894973</v>
-      </c>
-      <c r="E505" s="1">
-        <f>$J$499*L$507/L505*M505/M$507</f>
-        <v>798.00121499835893</v>
-      </c>
-      <c r="H505" s="1">
-        <f>C505+D505</f>
-        <v>510720.77759894973</v>
-      </c>
-      <c r="K505" s="1">
-        <v>1795</v>
-      </c>
-      <c r="L505" s="12">
-        <v>0.18</v>
-      </c>
-      <c r="M505" s="2">
-        <f t="shared" si="44"/>
-        <v>1.1609689553699984</v>
-      </c>
-      <c r="N505" s="1">
-        <v>15</v>
-      </c>
-      <c r="O505" s="1">
-        <f>$E$503*L$503/L505*M505/M$503</f>
-        <v>1704.1948442663563</v>
-      </c>
-    </row>
-    <row r="506" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A506" s="1">
-        <v>1796</v>
-      </c>
-      <c r="B506" s="1">
-        <f>B491*$D$499*$L$502/L506*M506</f>
-        <v>56381.045684836885</v>
-      </c>
-      <c r="C506" s="1">
-        <f>B506*$C$410</f>
-        <v>80823.292875032246</v>
-      </c>
-      <c r="D506" s="1">
-        <f>C506*0.15</f>
-        <v>12123.493931254836</v>
-      </c>
-      <c r="E506" s="1">
-        <f>(C506+D506)/B465</f>
-        <v>190.07522864271388</v>
-      </c>
-      <c r="F506" s="1">
-        <f>E506*L506/$L$507*M$507/M506</f>
-        <v>17.064531638145873</v>
-      </c>
-      <c r="H506" s="1">
-        <f>C506+D506</f>
-        <v>92946.786806287084</v>
-      </c>
-      <c r="K506" s="1">
-        <v>1796</v>
-      </c>
-      <c r="L506" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="M506" s="2">
-        <f t="shared" si="44"/>
-        <v>1.1725786449236988</v>
-      </c>
-      <c r="N506" s="1">
-        <v>16</v>
-      </c>
-      <c r="O506" s="1">
-        <f>$E$503*L$503/L506*M506/M$503</f>
-        <v>774.55655671905913</v>
-      </c>
-    </row>
-    <row r="507" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A507" s="1">
-        <v>1797</v>
-      </c>
-      <c r="B507" s="1">
-        <f>B492*$D$499*$L$502/L507*M507</f>
-        <v>16310.131635643185</v>
-      </c>
-      <c r="C507" s="1">
-        <f t="shared" ref="C507:C511" si="45">B507*$C$410</f>
-        <v>23380.881464787111</v>
-      </c>
-      <c r="D507" s="1">
-        <f t="shared" ref="D507:D511" si="46">C507*0.15</f>
-        <v>3507.1322197180666</v>
-      </c>
-      <c r="E507" s="1">
-        <f>(C507+D507)/B466</f>
-        <v>28.332996506327902</v>
-      </c>
-      <c r="F507" s="1">
-        <f t="shared" ref="F507:F524" si="47">E507*L507/$L$507*M$507/M507</f>
-        <v>28.332996506327898</v>
-      </c>
-      <c r="H507" s="1">
-        <f>C507+D507</f>
-        <v>26888.013684505178</v>
-      </c>
-      <c r="K507" s="1">
-        <v>1797</v>
-      </c>
-      <c r="L507" s="12">
+      <c r="L551" s="12">
         <v>4.5</v>
       </c>
-      <c r="M507" s="2">
-        <f t="shared" si="44"/>
-        <v>1.1843044313729358</v>
-      </c>
-      <c r="N507" s="1">
-        <v>17</v>
-      </c>
-      <c r="O507" s="1">
-        <f>$E$503*L$503/L507*M507/M$503</f>
-        <v>69.537966425444424</v>
-      </c>
-    </row>
-    <row r="508" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A508" s="1">
-        <v>1798</v>
-      </c>
-      <c r="B508" s="1">
-        <f>B493*$D$499*$L$502/L508*M508</f>
-        <v>16359.624448882381</v>
-      </c>
-      <c r="C508" s="1">
-        <f t="shared" si="45"/>
-        <v>23451.830346473365</v>
-      </c>
-      <c r="D508" s="1">
-        <f t="shared" si="46"/>
-        <v>3517.7745519710047</v>
-      </c>
-      <c r="E508" s="1">
-        <f t="shared" ref="E507:E515" si="48">(C508+D508)/B467</f>
-        <v>39.20000711983193</v>
-      </c>
-      <c r="F508" s="1">
-        <f t="shared" si="47"/>
-        <v>38.811888237457353</v>
-      </c>
-      <c r="H508" s="1">
-        <f>C508+D508</f>
-        <v>26969.60489844437</v>
-      </c>
-      <c r="K508" s="1">
-        <v>1798</v>
-      </c>
-      <c r="L508" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M508" s="2">
-        <f t="shared" si="44"/>
-        <v>1.1961474756866652</v>
-      </c>
-      <c r="N508" s="1">
-        <v>18</v>
-      </c>
-      <c r="O508" s="1">
-        <f>$E$503*L$503/L508*M508/M$503</f>
-        <v>70.23334608969887</v>
-      </c>
-    </row>
-    <row r="509" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A509" s="1">
-        <v>1799</v>
-      </c>
-      <c r="B509" s="1">
-        <f>B494*$D$499*$L$502/L509*M509</f>
-        <v>13425.116813364102</v>
-      </c>
-      <c r="C509" s="1">
-        <f t="shared" si="45"/>
-        <v>19245.158278074701</v>
-      </c>
-      <c r="D509" s="1">
-        <f t="shared" si="46"/>
-        <v>2886.7737417112053</v>
-      </c>
-      <c r="E509" s="1">
-        <f t="shared" si="48"/>
-        <v>30.31771509559713</v>
-      </c>
-      <c r="F509" s="1">
-        <f t="shared" si="47"/>
-        <v>29.720336335258441</v>
-      </c>
-      <c r="H509" s="1">
-        <f>C509+D509</f>
-        <v>22131.932019785905</v>
-      </c>
-      <c r="K509" s="1">
-        <v>1799</v>
-      </c>
-      <c r="L509" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M509" s="2">
-        <f t="shared" si="44"/>
-        <v>1.2081089504435316</v>
-      </c>
-      <c r="N509" s="1">
-        <v>19</v>
-      </c>
-      <c r="O509" s="1">
-        <f>$E$503*L$503/L509*M509/M$503</f>
-        <v>70.935679550595836</v>
-      </c>
-    </row>
-    <row r="510" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A510" s="1">
-        <v>1800</v>
-      </c>
-      <c r="B510" s="1">
-        <f>B495*$D$499*$L$502/L510*M510</f>
-        <v>10082.606960600884</v>
-      </c>
-      <c r="C510" s="1">
-        <f t="shared" si="45"/>
-        <v>14453.607332430973</v>
-      </c>
-      <c r="D510" s="1">
-        <f t="shared" si="46"/>
-        <v>2168.0410998646457</v>
-      </c>
-      <c r="E510" s="1">
-        <f t="shared" si="48"/>
-        <v>24.957430078521949</v>
-      </c>
-      <c r="F510" s="1">
-        <f t="shared" si="47"/>
-        <v>24.223435751806466</v>
-      </c>
-      <c r="H510" s="1">
-        <f>C510+D510</f>
-        <v>16621.648432295617</v>
-      </c>
-      <c r="K510" s="1">
-        <v>1800</v>
-      </c>
-      <c r="L510" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M510" s="2">
-        <f t="shared" si="44"/>
-        <v>1.220190039947967</v>
-      </c>
-      <c r="N510" s="1">
-        <v>20</v>
-      </c>
-      <c r="O510" s="1">
-        <f>$E$503*L$503/L510*M510/M$503</f>
-        <v>71.645036346101804</v>
-      </c>
-    </row>
-    <row r="511" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A511" s="1">
-        <v>1801</v>
-      </c>
-      <c r="B511" s="1">
-        <f>B496*$D$499*$L$502/L511*M511</f>
-        <v>6437.8024903606793</v>
-      </c>
-      <c r="C511" s="1">
-        <f t="shared" si="45"/>
-        <v>9228.7113484659822</v>
-      </c>
-      <c r="D511" s="1">
-        <f t="shared" si="46"/>
-        <v>1384.3067022698972</v>
-      </c>
-      <c r="E511" s="1">
-        <f t="shared" si="48"/>
-        <v>26.599042733673883</v>
-      </c>
-      <c r="F511" s="1">
-        <f t="shared" si="47"/>
-        <v>25.561157249119084</v>
-      </c>
-      <c r="H511" s="1">
-        <f>C511+D511</f>
-        <v>10613.01805073588</v>
-      </c>
-      <c r="K511" s="1">
-        <v>1801</v>
-      </c>
-      <c r="L511" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M511" s="2">
-        <f t="shared" si="44"/>
-        <v>1.2323919403474466</v>
-      </c>
-      <c r="N511" s="1">
-        <v>21</v>
-      </c>
-      <c r="O511" s="1">
-        <f>$E$503*L$503/L511*M511/M$503</f>
-        <v>72.361486709562811</v>
-      </c>
-    </row>
-    <row r="512" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A512" s="1">
-        <v>1802</v>
-      </c>
-      <c r="D512" s="1">
-        <f>B471*$J$502</f>
-        <v>0</v>
-      </c>
-      <c r="K512" s="1">
-        <v>1802</v>
-      </c>
-      <c r="L512" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M512" s="2">
-        <f t="shared" si="44"/>
-        <v>1.2447158597509214</v>
-      </c>
-      <c r="N512" s="1">
-        <v>22</v>
-      </c>
-      <c r="O512" s="1">
-        <f>$E$503*L$503/L512*M512/M$503</f>
-        <v>73.08510157665846</v>
-      </c>
-    </row>
-    <row r="513" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A513" s="1">
-        <v>1803</v>
-      </c>
-      <c r="B513" s="1">
-        <f>C513/(C$410)</f>
-        <v>4607.2827138017983</v>
-      </c>
-      <c r="C513" s="1">
-        <f>H513-D513</f>
-        <v>6604.6267076565209</v>
-      </c>
-      <c r="D513" s="1">
-        <f>O$501*H513</f>
-        <v>1068.7674771751956</v>
-      </c>
-      <c r="E513" s="1">
-        <f>$J$499*L$507/L513*M513/M$507</f>
-        <v>34.564838670413138</v>
-      </c>
-      <c r="F513" s="1">
-        <f t="shared" si="47"/>
-        <v>32.56164157679305</v>
-      </c>
-      <c r="H513" s="3">
-        <f>B472*E513</f>
-        <v>7673.3941848317163</v>
-      </c>
-      <c r="K513" s="1">
-        <v>1803</v>
-      </c>
-      <c r="L513" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M513" s="2">
-        <f t="shared" si="44"/>
-        <v>1.2571630183484304</v>
-      </c>
-      <c r="N513" s="1">
-        <v>23</v>
-      </c>
-      <c r="O513" s="1">
-        <f>$E$503*L$503/L513*M513/M$503</f>
-        <v>73.815952592425035</v>
-      </c>
-    </row>
-    <row r="514" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A514" s="1">
-        <v>1804</v>
-      </c>
-      <c r="B514" s="1">
-        <f t="shared" ref="B514:B524" si="49">C514/(C$410)</f>
-        <v>8111.9306051518442</v>
-      </c>
-      <c r="C514" s="1">
-        <f t="shared" ref="C514:C524" si="50">H514-D514</f>
-        <v>11628.605591088763</v>
-      </c>
-      <c r="D514" s="1">
-        <f t="shared" ref="D514:D524" si="51">O$501*H514</f>
-        <v>1881.7529000156255</v>
-      </c>
-      <c r="E514" s="1">
-        <f t="shared" ref="E514:E524" si="52">$J$499*L$507/L514*M514/M$507</f>
-        <v>34.91048705711728</v>
-      </c>
-      <c r="F514" s="1">
-        <f t="shared" si="47"/>
-        <v>32.56164157679305</v>
-      </c>
-      <c r="H514" s="3">
-        <f t="shared" ref="H514:H524" si="53">B473*E514</f>
-        <v>13510.358491104387</v>
-      </c>
-      <c r="L514" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M514" s="2">
-        <f t="shared" si="44"/>
-        <v>1.269734648531915</v>
-      </c>
-      <c r="N514" s="1">
-        <v>24</v>
-      </c>
-      <c r="O514" s="1">
-        <f>$E$503*L$503/L514*M514/M$503</f>
-        <v>74.554112118349295</v>
-      </c>
-    </row>
-    <row r="515" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A515" s="1">
-        <v>1805</v>
-      </c>
-      <c r="B515" s="1">
-        <f t="shared" si="49"/>
-        <v>10733.530503824561</v>
-      </c>
-      <c r="C515" s="1">
-        <f t="shared" si="50"/>
-        <v>15386.718514286364</v>
-      </c>
-      <c r="D515" s="1">
+      <c r="M551" s="2">
         <f t="shared" si="51"/>
-        <v>2489.8945930516829</v>
-      </c>
-      <c r="E515" s="1">
-        <f t="shared" si="52"/>
-        <v>35.259591927688454</v>
-      </c>
-      <c r="F515" s="1">
-        <f t="shared" si="47"/>
-        <v>32.56164157679305</v>
-      </c>
-      <c r="H515" s="3">
-        <f t="shared" si="53"/>
-        <v>17876.613107338046</v>
-      </c>
-      <c r="L515" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M515" s="2">
-        <f t="shared" si="44"/>
-        <v>1.2824319950172343</v>
-      </c>
-      <c r="N515" s="1">
-        <v>25</v>
-      </c>
-      <c r="O515" s="1">
-        <f>$E$503*L$503/L515*M515/M$503</f>
-        <v>75.299653239532802</v>
-      </c>
-    </row>
-    <row r="516" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A516" s="1">
-        <v>1806</v>
-      </c>
-      <c r="B516" s="1">
-        <f t="shared" si="49"/>
-        <v>11097.454348717545</v>
-      </c>
-      <c r="C516" s="1">
-        <f t="shared" si="50"/>
-        <v>15908.410213025183</v>
-      </c>
-      <c r="D516" s="1">
-        <f t="shared" si="51"/>
-        <v>2574.3152795498258</v>
-      </c>
-      <c r="E516" s="1">
-        <f t="shared" si="52"/>
-        <v>35.612187846965334</v>
-      </c>
-      <c r="F516" s="1">
-        <f t="shared" si="47"/>
-        <v>32.56164157679305</v>
-      </c>
-      <c r="H516" s="3">
-        <f t="shared" si="53"/>
-        <v>18482.725492575009</v>
-      </c>
-      <c r="L516" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M516" s="2">
-        <f t="shared" si="44"/>
-        <v>1.2952563149674066</v>
-      </c>
-      <c r="N516" s="1">
-        <v>26</v>
-      </c>
-      <c r="O516" s="1">
-        <f>$E$503*L$503/L516*M516/M$503</f>
-        <v>76.052649771928131</v>
-      </c>
-    </row>
-    <row r="517" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A517" s="1">
-        <v>1807</v>
-      </c>
-      <c r="B517" s="1">
-        <f t="shared" si="49"/>
-        <v>12072.276976382347</v>
-      </c>
-      <c r="C517" s="1">
-        <f t="shared" si="50"/>
-        <v>17305.836844261823</v>
-      </c>
-      <c r="D517" s="1">
-        <f t="shared" si="51"/>
-        <v>2800.4482922563307</v>
-      </c>
-      <c r="E517" s="1">
-        <f t="shared" si="52"/>
-        <v>35.968309725434978</v>
-      </c>
-      <c r="F517" s="1">
-        <f t="shared" si="47"/>
-        <v>32.56164157679305</v>
-      </c>
-      <c r="H517" s="3">
-        <f t="shared" si="53"/>
-        <v>20106.285136518152</v>
-      </c>
-      <c r="L517" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M517" s="2">
-        <f t="shared" si="44"/>
-        <v>1.3082088781170802</v>
-      </c>
-      <c r="N517" s="1">
-        <v>27</v>
-      </c>
-      <c r="O517" s="1">
-        <f>$E$503*L$503/L517*M517/M$503</f>
-        <v>76.813176269647386</v>
-      </c>
-    </row>
-    <row r="518" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A518" s="1">
-        <v>1808</v>
-      </c>
-      <c r="B518" s="1">
-        <f t="shared" si="49"/>
-        <v>10229.904974852512</v>
-      </c>
-      <c r="C518" s="1">
-        <f t="shared" si="50"/>
-        <v>14664.761815310168</v>
-      </c>
-      <c r="D518" s="1">
-        <f t="shared" si="51"/>
-        <v>2373.0668185311301</v>
-      </c>
-      <c r="E518" s="1">
-        <f t="shared" si="52"/>
-        <v>36.327992822689332</v>
-      </c>
-      <c r="F518" s="1">
-        <f t="shared" si="47"/>
-        <v>32.56164157679305</v>
-      </c>
-      <c r="H518" s="3">
-        <f t="shared" si="53"/>
-        <v>17037.828633841298</v>
-      </c>
-      <c r="L518" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M518" s="2">
-        <f t="shared" si="44"/>
-        <v>1.3212909668982511</v>
-      </c>
-      <c r="N518" s="1">
-        <v>28</v>
-      </c>
-      <c r="O518" s="1">
-        <f>$E$503*L$503/L518*M518/M$503</f>
-        <v>77.58130803234387</v>
-      </c>
-    </row>
-    <row r="519" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A519" s="1">
-        <v>1809</v>
-      </c>
-      <c r="B519" s="1">
-        <f t="shared" si="49"/>
-        <v>12579.293172808511</v>
-      </c>
-      <c r="C519" s="1">
-        <f t="shared" si="50"/>
-        <v>18032.654129013914</v>
-      </c>
-      <c r="D519" s="1">
-        <f t="shared" si="51"/>
-        <v>2918.0626117592492</v>
-      </c>
-      <c r="E519" s="1">
-        <f t="shared" si="52"/>
-        <v>36.691272750916227</v>
-      </c>
-      <c r="F519" s="1">
-        <f t="shared" si="47"/>
-        <v>32.56164157679305</v>
-      </c>
-      <c r="H519" s="3">
-        <f t="shared" si="53"/>
-        <v>20950.716740773165</v>
-      </c>
-      <c r="L519" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M519" s="2">
-        <f t="shared" si="44"/>
-        <v>1.3345038765672337</v>
-      </c>
-      <c r="N519" s="1">
-        <v>29</v>
-      </c>
-      <c r="O519" s="1">
-        <f>$E$503*L$503/L519*M519/M$503</f>
-        <v>78.357121112667315</v>
-      </c>
-    </row>
-    <row r="520" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A520" s="1">
-        <v>1810</v>
-      </c>
-      <c r="B520" s="1">
-        <f t="shared" si="49"/>
-        <v>13773.114358508155</v>
-      </c>
-      <c r="C520" s="1">
-        <f t="shared" si="50"/>
-        <v>19744.019325601075</v>
-      </c>
-      <c r="D520" s="1">
-        <f t="shared" si="51"/>
-        <v>3194.9974855442483</v>
-      </c>
-      <c r="E520" s="1">
-        <f t="shared" si="52"/>
-        <v>37.058185478425401</v>
-      </c>
-      <c r="F520" s="1">
-        <f t="shared" si="47"/>
-        <v>32.56164157679305</v>
-      </c>
-      <c r="H520" s="3">
-        <f t="shared" si="53"/>
-        <v>22939.016811145324</v>
-      </c>
-      <c r="L520" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M520" s="2">
-        <f t="shared" si="44"/>
-        <v>1.3478489153329063</v>
-      </c>
-      <c r="N520" s="1">
-        <v>30</v>
-      </c>
-      <c r="O520" s="1">
-        <f>$E$503*L$503/L520*M520/M$503</f>
-        <v>79.140692323793999</v>
-      </c>
-    </row>
-    <row r="521" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A521" s="1">
-        <v>1811</v>
-      </c>
-      <c r="B521" s="1">
-        <f t="shared" si="49"/>
-        <v>10562.354420006168</v>
-      </c>
-      <c r="C521" s="1">
-        <f t="shared" si="50"/>
-        <v>15141.33436811442</v>
-      </c>
-      <c r="D521" s="1">
-        <f t="shared" si="51"/>
-        <v>2450.1862784941095</v>
-      </c>
-      <c r="E521" s="1">
-        <f t="shared" si="52"/>
-        <v>37.428767333209635</v>
-      </c>
-      <c r="F521" s="1">
-        <f t="shared" si="47"/>
-        <v>32.56164157679305</v>
-      </c>
-      <c r="H521" s="3">
-        <f t="shared" si="53"/>
-        <v>17591.520646608529</v>
-      </c>
-      <c r="L521" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M521" s="2">
-        <f t="shared" si="44"/>
-        <v>1.3613274044862349</v>
-      </c>
-      <c r="N521" s="1">
-        <v>31</v>
-      </c>
-      <c r="O521" s="1">
-        <f>$E$503*L$503/L521*M521/M$503</f>
-        <v>79.932099247031914</v>
-      </c>
-    </row>
-    <row r="522" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A522" s="1">
-        <v>1812</v>
-      </c>
-      <c r="B522" s="1">
-        <f t="shared" si="49"/>
-        <v>10781.467091485021</v>
-      </c>
-      <c r="C522" s="1">
-        <f t="shared" si="50"/>
-        <v>15455.436517240201</v>
-      </c>
-      <c r="D522" s="1">
-        <f t="shared" si="51"/>
-        <v>2501.0146108671265</v>
-      </c>
-      <c r="E522" s="1">
-        <f t="shared" si="52"/>
-        <v>37.80305500654174</v>
-      </c>
-      <c r="F522" s="1">
-        <f t="shared" si="47"/>
-        <v>32.561641576793043</v>
-      </c>
-      <c r="H522" s="3">
-        <f t="shared" si="53"/>
-        <v>17956.451128107328</v>
-      </c>
-      <c r="L522" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M522" s="2">
-        <f t="shared" si="44"/>
-        <v>1.3749406785310976</v>
-      </c>
-      <c r="N522" s="1">
-        <v>32</v>
-      </c>
-      <c r="O522" s="1">
-        <f>$E$503*L$503/L522*M522/M$503</f>
-        <v>80.731420239502256</v>
-      </c>
-    </row>
-    <row r="523" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A523" s="1">
-        <v>1813</v>
-      </c>
-      <c r="B523" s="1">
-        <f t="shared" si="49"/>
-        <v>8505.102176527058</v>
-      </c>
-      <c r="C523" s="1">
-        <f t="shared" si="50"/>
-        <v>12192.224457631739</v>
-      </c>
-      <c r="D523" s="1">
-        <f t="shared" si="51"/>
-        <v>1972.9582838695178</v>
-      </c>
-      <c r="E523" s="1">
-        <f t="shared" si="52"/>
-        <v>38.181085556607165</v>
-      </c>
-      <c r="F523" s="1">
-        <f t="shared" si="47"/>
-        <v>32.56164157679305</v>
-      </c>
-      <c r="H523" s="3">
-        <f t="shared" si="53"/>
-        <v>14165.182741501258</v>
-      </c>
-      <c r="L523" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M523" s="2">
-        <f t="shared" si="44"/>
-        <v>1.3886900853164086</v>
-      </c>
-      <c r="N523" s="1">
-        <v>33</v>
-      </c>
-      <c r="O523" s="1">
-        <f>$E$503*L$503/L523*M523/M$503</f>
-        <v>81.538734441897276</v>
-      </c>
-    </row>
-    <row r="524" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A524" s="1">
-        <v>1814</v>
-      </c>
-      <c r="B524" s="1">
-        <f t="shared" si="49"/>
-        <v>3357.3375033757084</v>
-      </c>
-      <c r="C524" s="1">
-        <f t="shared" si="50"/>
-        <v>4812.8066625880547</v>
-      </c>
-      <c r="D524" s="1">
-        <f t="shared" si="51"/>
-        <v>778.81331717706439</v>
-      </c>
-      <c r="E524" s="1">
-        <f t="shared" si="52"/>
-        <v>38.562896412173231</v>
-      </c>
-      <c r="F524" s="1">
-        <f t="shared" si="47"/>
-        <v>32.561641576793043</v>
-      </c>
-      <c r="H524" s="3">
-        <f t="shared" si="53"/>
-        <v>5591.6199797651188</v>
-      </c>
-      <c r="L524" s="12">
-        <v>4.5</v>
-      </c>
-      <c r="M524" s="2">
-        <f t="shared" si="44"/>
-        <v>1.4025769861695727</v>
-      </c>
-      <c r="N524" s="1">
-        <v>34</v>
-      </c>
-      <c r="O524" s="1">
-        <f>$E$503*L$503/L524*M524/M$503</f>
-        <v>82.354121786316242</v>
+        <v>1.4166027560312682</v>
+      </c>
+      <c r="N551" s="1">
+        <v>35</v>
+      </c>
+      <c r="O551" s="1">
+        <f>$E$529*L$529/L551*M551/M$529</f>
+        <v>114.68435353606552</v>
       </c>
     </row>
   </sheetData>
@@ -9098,10 +9370,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F52ADF-FFA8-0A46-9CC0-C7AD4F73CE98}">
-  <dimension ref="A1:G128"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10196,42 +10468,62 @@
         <v>1793</v>
       </c>
       <c r="B107" s="1">
-        <f>Calcul!C503</f>
-        <v>54463.697651335431</v>
+        <f>Calcul!C529</f>
+        <v>75093.886155629138</v>
       </c>
       <c r="C107" s="1">
-        <f>Calcul!B503</f>
-        <v>37993.010631143021</v>
+        <f>Calcul!B529</f>
+        <v>52384.302536878997</v>
       </c>
       <c r="D107">
-        <f t="shared" ref="D107:D128" si="5">(B107-C107)/C107</f>
-        <v>0.4335188695652174</v>
+        <f t="shared" ref="D107:D129" si="5">(B107-C107)/C107</f>
+        <v>0.43351886956521757</v>
       </c>
       <c r="E107" s="1">
-        <f>Calcul!D503</f>
-        <v>8169.5546477003145</v>
+        <f>Calcul!D529</f>
+        <v>11264.082923344371</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>1794</v>
       </c>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
+      <c r="B108" s="1">
+        <f>Calcul!C530</f>
+        <v>3939.99090998366</v>
+      </c>
+      <c r="C108" s="1">
+        <f>Calcul!B530</f>
+        <v>2748.4750941427433</v>
+      </c>
+      <c r="D108">
+        <f t="shared" ref="D108:D109" si="6">(B108-C108)/C108</f>
+        <v>0.43351886956521746</v>
+      </c>
       <c r="E108" s="1">
-        <f>Calcul!D504</f>
-        <v>64047.84382926664</v>
+        <f>Calcul!D530</f>
+        <v>590.998636497549</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>1795</v>
       </c>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
+      <c r="B109" s="1">
+        <f>Calcul!C531</f>
+        <v>90890.391694205682</v>
+      </c>
+      <c r="C109" s="1">
+        <f>Calcul!B531</f>
+        <v>63403.693961679419</v>
+      </c>
+      <c r="D109">
+        <f>(B109-C109)/C109</f>
+        <v>0.4335188695652174</v>
+      </c>
       <c r="E109" s="1">
-        <f>Calcul!D505</f>
-        <v>510720.77759894973</v>
+        <f>Calcul!D531</f>
+        <v>13633.558754130852</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
@@ -10239,20 +10531,20 @@
         <v>1796</v>
       </c>
       <c r="B110" s="1">
-        <f>Calcul!C506</f>
-        <v>80823.292875032246</v>
+        <f>Calcul!C532</f>
+        <v>235285.58592509385</v>
       </c>
       <c r="C110" s="1">
-        <f>Calcul!B506</f>
-        <v>56381.045684836885</v>
+        <f>Calcul!B532</f>
+        <v>164131.4885491918</v>
       </c>
       <c r="D110">
         <f t="shared" si="5"/>
-        <v>0.43351886956521735</v>
+        <v>0.43351886956521746</v>
       </c>
       <c r="E110" s="1">
-        <f>Calcul!D506</f>
-        <v>12123.493931254836</v>
+        <f>Calcul!D532</f>
+        <v>35292.837888764079</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
@@ -10260,20 +10552,20 @@
         <v>1797</v>
       </c>
       <c r="B111" s="1">
-        <f>Calcul!C507</f>
-        <v>23380.881464787111</v>
+        <f>Calcul!C533</f>
+        <v>50309.207013886757</v>
       </c>
       <c r="C111" s="1">
-        <f>Calcul!B507</f>
-        <v>16310.131635643185</v>
+        <f>Calcul!B533</f>
+        <v>35094.903933246031</v>
       </c>
       <c r="D111">
         <f t="shared" si="5"/>
         <v>0.43351886956521751</v>
       </c>
       <c r="E111" s="1">
-        <f>Calcul!D507</f>
-        <v>3507.1322197180666</v>
+        <f>Calcul!D533</f>
+        <v>7546.3810520830129</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
@@ -10281,20 +10573,20 @@
         <v>1798</v>
       </c>
       <c r="B112" s="1">
-        <f>Calcul!C508</f>
-        <v>23451.830346473365</v>
+        <f>Calcul!C534</f>
+        <v>44949.34149740728</v>
       </c>
       <c r="C112" s="1">
-        <f>Calcul!B508</f>
-        <v>16359.624448882381</v>
+        <f>Calcul!B534</f>
+        <v>31355.946860357893</v>
       </c>
       <c r="D112">
         <f t="shared" si="5"/>
-        <v>0.43351886956521746</v>
+        <v>0.43351886956521757</v>
       </c>
       <c r="E112" s="1">
-        <f>Calcul!D508</f>
-        <v>3517.7745519710047</v>
+        <f>Calcul!D534</f>
+        <v>6742.4012246110915</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -10302,20 +10594,20 @@
         <v>1799</v>
       </c>
       <c r="B113" s="1">
-        <f>Calcul!C509</f>
-        <v>19245.158278074701</v>
+        <f>Calcul!C535</f>
+        <v>32404.240861373633</v>
       </c>
       <c r="C113" s="1">
-        <f>Calcul!B509</f>
-        <v>13425.116813364102</v>
+        <f>Calcul!B535</f>
+        <v>22604.683865236984</v>
       </c>
       <c r="D113">
         <f t="shared" si="5"/>
-        <v>0.4335188695652174</v>
+        <v>0.43351886956521751</v>
       </c>
       <c r="E113" s="1">
-        <f>Calcul!D509</f>
-        <v>2886.7737417112053</v>
+        <f>Calcul!D535</f>
+        <v>4860.6361292060446</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -10323,20 +10615,20 @@
         <v>1800</v>
       </c>
       <c r="B114" s="1">
-        <f>Calcul!C510</f>
-        <v>14453.607332430973</v>
+        <f>Calcul!C536</f>
+        <v>23923.212136437476</v>
       </c>
       <c r="C114" s="1">
-        <f>Calcul!B510</f>
-        <v>10082.606960600884</v>
+        <f>Calcul!B536</f>
+        <v>16688.452900304914</v>
       </c>
       <c r="D114">
         <f t="shared" si="5"/>
-        <v>0.43351886956521751</v>
+        <v>0.43351886956521757</v>
       </c>
       <c r="E114" s="1">
-        <f>Calcul!D510</f>
-        <v>2168.0410998646457</v>
+        <f>Calcul!D536</f>
+        <v>3588.4818204656212</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -10344,48 +10636,62 @@
         <v>1801</v>
       </c>
       <c r="B115" s="1">
-        <f>Calcul!C511</f>
-        <v>9228.7113484659822</v>
+        <f>Calcul!C537</f>
+        <v>14598.143405755281</v>
       </c>
       <c r="C115" s="1">
-        <f>Calcul!B511</f>
-        <v>6437.8024903606793</v>
+        <f>Calcul!B537</f>
+        <v>10183.433030206892</v>
       </c>
       <c r="D115">
         <f t="shared" si="5"/>
-        <v>0.4335188695652174</v>
+        <v>0.43351886956521751</v>
       </c>
       <c r="E115" s="1">
-        <f>Calcul!D511</f>
-        <v>1384.3067022698972</v>
+        <f>Calcul!D537</f>
+        <v>2189.7215108632922</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>1802</v>
       </c>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1"/>
+      <c r="B116" s="1">
+        <f>Calcul!C538</f>
+        <v>677.89079723277416</v>
+      </c>
+      <c r="C116" s="1">
+        <f>Calcul!B538</f>
+        <v>472.88585565558458</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="5"/>
+        <v>0.4335188695652174</v>
+      </c>
+      <c r="E116" s="1">
+        <f>Calcul!D538</f>
+        <v>101.68361958491612</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>1803</v>
       </c>
       <c r="B117" s="1">
-        <f>Calcul!C513</f>
-        <v>6604.6267076565209</v>
+        <f>Calcul!C539</f>
+        <v>13179.89182519821</v>
       </c>
       <c r="C117" s="1">
-        <f>Calcul!B513</f>
-        <v>4607.2827138017983</v>
+        <f>Calcul!B539</f>
+        <v>9194.0832485837018</v>
       </c>
       <c r="D117">
         <f t="shared" si="5"/>
-        <v>0.4335188695652174</v>
+        <v>0.43351886956521746</v>
       </c>
       <c r="E117" s="1">
-        <f>Calcul!D513</f>
-        <v>1068.7674771751956</v>
+        <f>Calcul!D539</f>
+        <v>1976.9837737797316</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -10393,20 +10699,20 @@
         <v>1804</v>
       </c>
       <c r="B118" s="1">
-        <f>Calcul!C514</f>
-        <v>11628.605591088763</v>
+        <f>Calcul!C540</f>
+        <v>6223.6476203143775</v>
       </c>
       <c r="C118" s="1">
-        <f>Calcul!B514</f>
-        <v>8111.9306051518442</v>
+        <f>Calcul!B540</f>
+        <v>4341.517752188357</v>
       </c>
       <c r="D118">
         <f t="shared" si="5"/>
-        <v>0.43351886956521751</v>
+        <v>0.43351886956521746</v>
       </c>
       <c r="E118" s="1">
-        <f>Calcul!D514</f>
-        <v>1881.7529000156255</v>
+        <f>Calcul!D540</f>
+        <v>933.54714304715662</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -10414,20 +10720,20 @@
         <v>1805</v>
       </c>
       <c r="B119" s="1">
-        <f>Calcul!C515</f>
-        <v>15386.718514286364</v>
+        <f>Calcul!C541</f>
+        <v>5238.2367470979352</v>
       </c>
       <c r="C119" s="1">
-        <f>Calcul!B515</f>
-        <v>10733.530503824561</v>
+        <f>Calcul!B541</f>
+        <v>3654.1107747585343</v>
       </c>
       <c r="D119">
         <f t="shared" si="5"/>
         <v>0.43351886956521751</v>
       </c>
       <c r="E119" s="1">
-        <f>Calcul!D515</f>
-        <v>2489.8945930516829</v>
+        <f>Calcul!D541</f>
+        <v>785.73551206469028</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -10435,20 +10741,20 @@
         <v>1806</v>
       </c>
       <c r="B120" s="1">
-        <f>Calcul!C516</f>
-        <v>15908.410213025183</v>
+        <f>Calcul!C542</f>
+        <v>10404.884258652197</v>
       </c>
       <c r="C120" s="1">
-        <f>Calcul!B516</f>
-        <v>11097.454348717545</v>
+        <f>Calcul!B542</f>
+        <v>7258.2820355953681</v>
       </c>
       <c r="D120">
         <f t="shared" si="5"/>
-        <v>0.43351886956521757</v>
+        <v>0.43351886956521735</v>
       </c>
       <c r="E120" s="1">
-        <f>Calcul!D516</f>
-        <v>2574.3152795498258</v>
+        <f>Calcul!D542</f>
+        <v>1560.7326387978294</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -10456,20 +10762,20 @@
         <v>1807</v>
       </c>
       <c r="B121" s="1">
-        <f>Calcul!C517</f>
-        <v>17305.836844261823</v>
+        <f>Calcul!C543</f>
+        <v>17099.280978286723</v>
       </c>
       <c r="C121" s="1">
-        <f>Calcul!B517</f>
-        <v>12072.276976382347</v>
+        <f>Calcul!B543</f>
+        <v>11928.186884259772</v>
       </c>
       <c r="D121">
         <f t="shared" si="5"/>
-        <v>0.4335188695652174</v>
+        <v>0.43351886956521746</v>
       </c>
       <c r="E121" s="1">
-        <f>Calcul!D517</f>
-        <v>2800.4482922563307</v>
+        <f>Calcul!D543</f>
+        <v>2564.8921467430082</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -10477,20 +10783,20 @@
         <v>1808</v>
       </c>
       <c r="B122" s="1">
-        <f>Calcul!C518</f>
-        <v>14664.761815310168</v>
+        <f>Calcul!C544</f>
+        <v>27344.600164443524</v>
       </c>
       <c r="C122" s="1">
-        <f>Calcul!B518</f>
-        <v>10229.904974852512</v>
+        <f>Calcul!B544</f>
+        <v>19075.158859078758</v>
       </c>
       <c r="D122">
         <f t="shared" si="5"/>
-        <v>0.43351886956521757</v>
+        <v>0.43351886956521746</v>
       </c>
       <c r="E122" s="1">
-        <f>Calcul!D518</f>
-        <v>2373.0668185311301</v>
+        <f>Calcul!D544</f>
+        <v>4101.6900246665282</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -10498,20 +10804,20 @@
         <v>1809</v>
       </c>
       <c r="B123" s="1">
-        <f>Calcul!C519</f>
-        <v>18032.654129013914</v>
+        <f>Calcul!C545</f>
+        <v>30525.208920413002</v>
       </c>
       <c r="C123" s="1">
-        <f>Calcul!B519</f>
-        <v>12579.293172808511</v>
+        <f>Calcul!B545</f>
+        <v>21293.901021108442</v>
       </c>
       <c r="D123">
         <f t="shared" si="5"/>
         <v>0.4335188695652174</v>
       </c>
       <c r="E123" s="1">
-        <f>Calcul!D519</f>
-        <v>2918.0626117592492</v>
+        <f>Calcul!D545</f>
+        <v>4578.78133806195</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -10519,20 +10825,20 @@
         <v>1810</v>
       </c>
       <c r="B124" s="1">
-        <f>Calcul!C520</f>
-        <v>19744.019325601075</v>
+        <f>Calcul!C546</f>
+        <v>38538.07626202143</v>
       </c>
       <c r="C124" s="1">
-        <f>Calcul!B520</f>
-        <v>13773.114358508155</v>
+        <f>Calcul!B546</f>
+        <v>26883.550039149417</v>
       </c>
       <c r="D124">
         <f t="shared" si="5"/>
-        <v>0.4335188695652174</v>
+        <v>0.43351886956521746</v>
       </c>
       <c r="E124" s="1">
-        <f>Calcul!D520</f>
-        <v>3194.9974855442483</v>
+        <f>Calcul!D546</f>
+        <v>5780.7114393032143</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -10540,20 +10846,20 @@
         <v>1811</v>
       </c>
       <c r="B125" s="1">
-        <f>Calcul!C521</f>
-        <v>15141.33436811442</v>
+        <f>Calcul!C547</f>
+        <v>40035.555796774242</v>
       </c>
       <c r="C125" s="1">
-        <f>Calcul!B521</f>
-        <v>10562.354420006168</v>
+        <f>Calcul!B547</f>
+        <v>27928.167983527783</v>
       </c>
       <c r="D125">
         <f t="shared" si="5"/>
-        <v>0.43351886956521746</v>
+        <v>0.43351886956521735</v>
       </c>
       <c r="E125" s="1">
-        <f>Calcul!D521</f>
-        <v>2450.1862784941095</v>
+        <f>Calcul!D547</f>
+        <v>6005.3333695161364</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -10561,20 +10867,20 @@
         <v>1812</v>
       </c>
       <c r="B126" s="1">
-        <f>Calcul!C522</f>
-        <v>15455.436517240201</v>
+        <f>Calcul!C548</f>
+        <v>15725.076637955222</v>
       </c>
       <c r="C126" s="1">
-        <f>Calcul!B522</f>
-        <v>10781.467091485021</v>
+        <f>Calcul!B548</f>
+        <v>10969.563757974527</v>
       </c>
       <c r="D126">
         <f t="shared" si="5"/>
-        <v>0.43351886956521751</v>
+        <v>0.4335188695652174</v>
       </c>
       <c r="E126" s="1">
-        <f>Calcul!D522</f>
-        <v>2501.0146108671265</v>
+        <f>Calcul!D548</f>
+        <v>2358.7614956932835</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -10582,20 +10888,20 @@
         <v>1813</v>
       </c>
       <c r="B127" s="1">
-        <f>Calcul!C523</f>
-        <v>12192.224457631739</v>
+        <f>Calcul!C549</f>
+        <v>14558.80012064021</v>
       </c>
       <c r="C127" s="1">
-        <f>Calcul!B523</f>
-        <v>8505.102176527058</v>
+        <f>Calcul!B549</f>
+        <v>10155.987779258083</v>
       </c>
       <c r="D127">
         <f t="shared" si="5"/>
-        <v>0.43351886956521746</v>
+        <v>0.4335188695652174</v>
       </c>
       <c r="E127" s="1">
-        <f>Calcul!D523</f>
-        <v>1972.9582838695178</v>
+        <f>Calcul!D549</f>
+        <v>2183.8200180960312</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -10603,20 +10909,41 @@
         <v>1814</v>
       </c>
       <c r="B128" s="1">
-        <f>Calcul!C524</f>
-        <v>4812.8066625880547</v>
+        <f>Calcul!C550</f>
+        <v>4774.1519876125367</v>
       </c>
       <c r="C128" s="1">
-        <f>Calcul!B524</f>
-        <v>3357.3375033757084</v>
+        <f>Calcul!B550</f>
+        <v>3330.3726159255402</v>
       </c>
       <c r="D128">
         <f t="shared" si="5"/>
-        <v>0.4335188695652174</v>
+        <v>0.43351886956521751</v>
       </c>
       <c r="E128" s="1">
-        <f>Calcul!D524</f>
-        <v>778.81331717706439</v>
+        <f>Calcul!D550</f>
+        <v>716.12279814188048</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>1815</v>
+      </c>
+      <c r="B129" s="1">
+        <f>Calcul!C551</f>
+        <v>192.87574029954644</v>
+      </c>
+      <c r="C129" s="1">
+        <f>Calcul!B551</f>
+        <v>134.54705368339179</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="5"/>
+        <v>0.43351886956521746</v>
+      </c>
+      <c r="E129" s="1">
+        <f>Calcul!D551</f>
+        <v>28.931361044931965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Explication des chiffres français de prédation
… Durant les Guerres de la Révolution et de l’Empire

Signed-off-by: Guillaume Daudin <gdaudin@mac.com>
</commit_message>
<xml_diff>
--- a/External Data/Résultats de la course française.xlsx
+++ b/External Data/Résultats de la course française.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumedaudin/Répertoires Git/2016-Hamburg-Impact-of-War/External Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEB8D32-25DB-F147-858E-FEF2A55369E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932F7EB6-FEC4-9C42-9697-E7C44A25A1BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="-14620" windowWidth="26880" windowHeight="14620" activeTab="1" xr2:uid="{E3D52932-A783-EC49-8617-8937D12F747E}"/>
+    <workbookView xWindow="1940" yWindow="1980" windowWidth="26880" windowHeight="14620" activeTab="1" xr2:uid="{E3D52932-A783-EC49-8617-8937D12F747E}"/>
   </bookViews>
   <sheets>
     <sheet name="Calcul" sheetId="1" r:id="rId1"/>
@@ -1176,7 +1176,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1195,6 +1195,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1209,7 +1215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1228,6 +1234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
@@ -1565,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747C72A1-6A8D-9E42-88DE-481B3F912E70}">
   <dimension ref="A1:O551"/>
   <sheetViews>
-    <sheetView topLeftCell="A527" workbookViewId="0">
-      <selection activeCell="H539" sqref="H539"/>
+    <sheetView topLeftCell="A516" workbookViewId="0">
+      <selection activeCell="H529" sqref="H529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8373,11 +8380,11 @@
         <f>C529*0.15</f>
         <v>11264.082923344371</v>
       </c>
-      <c r="E529" s="1">
+      <c r="E529" s="16">
         <f>(C529+D529)/B462</f>
         <v>245.33513942890201</v>
       </c>
-      <c r="F529" s="1">
+      <c r="F529" s="16">
         <f>E529*L529/$L$533*M529/M$533</f>
         <v>88.541821576798412</v>
       </c>
@@ -8408,27 +8415,27 @@
         <v>1794</v>
       </c>
       <c r="B530" s="1">
-        <f t="shared" ref="B530:B551" si="45">B500*$D$525*$L$528/L530*M530</f>
+        <f>B500*$D$525*$L$528/L530*M530</f>
         <v>2748.4750941427433</v>
       </c>
       <c r="C530" s="1">
-        <f t="shared" ref="C530:C551" si="46">B530*$C$410</f>
+        <f t="shared" ref="C530:C551" si="45">B530*$C$410</f>
         <v>3939.99090998366</v>
       </c>
       <c r="D530" s="1">
-        <f t="shared" ref="D530:D551" si="47">C530*0.15</f>
+        <f>C530*0.15</f>
         <v>590.998636497549</v>
       </c>
-      <c r="E530" s="1">
-        <f t="shared" ref="E530:E551" si="48">(C530+D530)/B463</f>
+      <c r="E530" s="16">
+        <f>(C530+D530)/B463</f>
         <v>7.0356980535422498</v>
       </c>
-      <c r="F530" s="1">
-        <f t="shared" ref="F530:F550" si="49">E530*L530/$L$533*M530/M$533</f>
+      <c r="F530" s="16">
+        <f>E530*L530/$L$533*M530/M$533</f>
         <v>2.1700342837385316</v>
       </c>
       <c r="H530" s="1">
-        <f t="shared" ref="H530:H550" si="50">C530+D530</f>
+        <f>C530+D530</f>
         <v>4530.9895464812089</v>
       </c>
       <c r="K530" s="1">
@@ -8438,14 +8445,14 @@
         <v>1.43</v>
       </c>
       <c r="M530" s="2">
-        <f t="shared" ref="M530:M551" si="51">(1+0.01)^N530</f>
+        <f t="shared" ref="M530:M551" si="46">(1+0.01)^N530</f>
         <v>1.1494742132376226</v>
       </c>
       <c r="N530" s="1">
         <v>14</v>
       </c>
       <c r="O530" s="1">
-        <f t="shared" ref="O530:O550" si="52">$E$529*L$529/L530*M530/M$529</f>
+        <f t="shared" ref="O530:O549" si="47">$E$529*L$529/L530*M530/M$529</f>
         <v>292.84094370013491</v>
       </c>
     </row>
@@ -8454,27 +8461,27 @@
         <v>1795</v>
       </c>
       <c r="B531" s="1">
+        <f t="shared" ref="B530:B550" si="48">B501*$D$525*$L$528/L531*M531</f>
+        <v>63403.693961679419</v>
+      </c>
+      <c r="C531" s="1">
         <f t="shared" si="45"/>
-        <v>63403.693961679419</v>
-      </c>
-      <c r="C531" s="1">
-        <f t="shared" si="46"/>
         <v>90890.391694205682</v>
       </c>
       <c r="D531" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" ref="D530:D551" si="49">C531*0.15</f>
         <v>13633.558754130852</v>
       </c>
-      <c r="E531" s="1">
-        <f t="shared" si="48"/>
+      <c r="E531" s="16">
+        <f t="shared" ref="E530:E550" si="50">(C531+D531)/B464</f>
         <v>163.31867257552582</v>
       </c>
-      <c r="F531" s="1">
-        <f t="shared" si="49"/>
+      <c r="F531" s="16">
+        <f t="shared" ref="F530:F550" si="51">E531*L531/$L$533*M531/M$533</f>
         <v>6.4040259808068134</v>
       </c>
       <c r="H531" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" ref="H530:H550" si="52">C531+D531</f>
         <v>104523.95044833653</v>
       </c>
       <c r="K531" s="1">
@@ -8484,14 +8491,14 @@
         <v>0.18</v>
       </c>
       <c r="M531" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.1609689553699984</v>
       </c>
       <c r="N531" s="1">
         <v>15</v>
       </c>
       <c r="O531" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>2349.7231943672487</v>
       </c>
     </row>
@@ -8500,27 +8507,27 @@
         <v>1796</v>
       </c>
       <c r="B532" s="1">
+        <f t="shared" si="48"/>
+        <v>164131.4885491918</v>
+      </c>
+      <c r="C532" s="1">
         <f t="shared" si="45"/>
-        <v>164131.4885491918</v>
-      </c>
-      <c r="C532" s="1">
-        <f t="shared" si="46"/>
         <v>235285.58592509385</v>
       </c>
       <c r="D532" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>35292.837888764079</v>
       </c>
-      <c r="E532" s="1">
-        <f t="shared" si="48"/>
+      <c r="E532" s="16">
+        <f t="shared" si="50"/>
         <v>553.33011004878927</v>
       </c>
-      <c r="F532" s="1">
-        <f t="shared" si="49"/>
+      <c r="F532" s="16">
+        <f t="shared" si="51"/>
         <v>48.697919476241076</v>
       </c>
       <c r="H532" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>270578.42381385795</v>
       </c>
       <c r="K532" s="1">
@@ -8530,14 +8537,14 @@
         <v>0.4</v>
       </c>
       <c r="M532" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.1725786449236988</v>
       </c>
       <c r="N532" s="1">
         <v>16</v>
       </c>
       <c r="O532" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>1067.9491918399146</v>
       </c>
     </row>
@@ -8546,27 +8553,27 @@
         <v>1797</v>
       </c>
       <c r="B533" s="1">
+        <f t="shared" si="48"/>
+        <v>35094.903933246031</v>
+      </c>
+      <c r="C533" s="1">
         <f t="shared" si="45"/>
-        <v>35094.903933246031</v>
-      </c>
-      <c r="C533" s="1">
-        <f t="shared" si="46"/>
         <v>50309.207013886757</v>
       </c>
       <c r="D533" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>7546.3810520830129</v>
       </c>
-      <c r="E533" s="1">
-        <f t="shared" si="48"/>
+      <c r="E533" s="16">
+        <f t="shared" si="50"/>
         <v>60.964792482581423</v>
       </c>
-      <c r="F533" s="1">
-        <f t="shared" si="49"/>
+      <c r="F533" s="16">
+        <f t="shared" si="51"/>
         <v>60.96479248258143</v>
       </c>
       <c r="H533" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>57855.588065969772</v>
       </c>
       <c r="K533" s="1">
@@ -8576,14 +8583,14 @@
         <v>4.5</v>
       </c>
       <c r="M533" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.1843044313729358</v>
       </c>
       <c r="N533" s="1">
         <v>17</v>
       </c>
       <c r="O533" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>95.878105222961238</v>
       </c>
     </row>
@@ -8592,27 +8599,27 @@
         <v>1798</v>
       </c>
       <c r="B534" s="1">
+        <f t="shared" si="48"/>
+        <v>31355.946860357893</v>
+      </c>
+      <c r="C534" s="1">
         <f t="shared" si="45"/>
-        <v>31355.946860357893</v>
-      </c>
-      <c r="C534" s="1">
-        <f t="shared" si="46"/>
         <v>44949.34149740728</v>
       </c>
       <c r="D534" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>6742.4012246110915</v>
       </c>
-      <c r="E534" s="1">
-        <f t="shared" si="48"/>
+      <c r="E534" s="16">
+        <f t="shared" si="50"/>
         <v>75.133346979677867</v>
       </c>
-      <c r="F534" s="1">
-        <f t="shared" si="49"/>
+      <c r="F534" s="16">
+        <f t="shared" si="51"/>
         <v>75.884680449474658</v>
       </c>
       <c r="H534" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>51691.742722018374</v>
       </c>
       <c r="K534" s="1">
@@ -8622,14 +8629,14 @@
         <v>4.5</v>
       </c>
       <c r="M534" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.1961474756866652</v>
       </c>
       <c r="N534" s="1">
         <v>18</v>
       </c>
       <c r="O534" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>96.836886275190849</v>
       </c>
     </row>
@@ -8638,27 +8645,27 @@
         <v>1799</v>
       </c>
       <c r="B535" s="1">
+        <f t="shared" si="48"/>
+        <v>22604.683865236984</v>
+      </c>
+      <c r="C535" s="1">
         <f t="shared" si="45"/>
-        <v>22604.683865236984</v>
-      </c>
-      <c r="C535" s="1">
-        <f t="shared" si="46"/>
         <v>32404.240861373633</v>
       </c>
       <c r="D535" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>4860.6361292060446</v>
       </c>
-      <c r="E535" s="1">
-        <f t="shared" si="48"/>
+      <c r="E535" s="16">
+        <f t="shared" si="50"/>
         <v>51.047776699424219</v>
       </c>
-      <c r="F535" s="1">
-        <f t="shared" si="49"/>
+      <c r="F535" s="16">
+        <f t="shared" si="51"/>
         <v>52.073837011082631</v>
       </c>
       <c r="H535" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>37264.87699057968</v>
       </c>
       <c r="K535" s="1">
@@ -8668,14 +8675,14 @@
         <v>4.5</v>
       </c>
       <c r="M535" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.2081089504435316</v>
       </c>
       <c r="N535" s="1">
         <v>19</v>
       </c>
       <c r="O535" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>97.805255137942737</v>
       </c>
     </row>
@@ -8684,27 +8691,27 @@
         <v>1800</v>
       </c>
       <c r="B536" s="1">
+        <f t="shared" si="48"/>
+        <v>16688.452900304914</v>
+      </c>
+      <c r="C536" s="1">
         <f t="shared" si="45"/>
-        <v>16688.452900304914</v>
-      </c>
-      <c r="C536" s="1">
-        <f t="shared" si="46"/>
         <v>23923.212136437476</v>
       </c>
       <c r="D536" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>3588.4818204656212</v>
       </c>
-      <c r="E536" s="1">
-        <f t="shared" si="48"/>
+      <c r="E536" s="16">
+        <f t="shared" si="50"/>
         <v>41.308849785139785</v>
       </c>
-      <c r="F536" s="1">
-        <f t="shared" si="49"/>
+      <c r="F536" s="16">
+        <f t="shared" si="51"/>
         <v>42.560549242479304</v>
       </c>
       <c r="H536" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>27511.693956903098</v>
       </c>
       <c r="K536" s="1">
@@ -8714,14 +8721,14 @@
         <v>4.5</v>
       </c>
       <c r="M536" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.220190039947967</v>
       </c>
       <c r="N536" s="1">
         <v>20</v>
       </c>
       <c r="O536" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>98.783307689322172</v>
       </c>
     </row>
@@ -8730,27 +8737,27 @@
         <v>1801</v>
       </c>
       <c r="B537" s="1">
+        <f t="shared" si="48"/>
+        <v>10183.433030206892</v>
+      </c>
+      <c r="C537" s="1">
         <f t="shared" si="45"/>
-        <v>10183.433030206892</v>
-      </c>
-      <c r="C537" s="1">
-        <f t="shared" si="46"/>
         <v>14598.143405755281</v>
       </c>
       <c r="D537" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>2189.7215108632922</v>
       </c>
-      <c r="E537" s="1">
-        <f t="shared" si="48"/>
+      <c r="E537" s="16">
+        <f t="shared" si="50"/>
         <v>42.074849415084145</v>
       </c>
-      <c r="F537" s="1">
-        <f t="shared" si="49"/>
+      <c r="F537" s="16">
+        <f t="shared" si="51"/>
         <v>43.783257021482704</v>
       </c>
       <c r="H537" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>16787.864916618575</v>
       </c>
       <c r="K537" s="1">
@@ -8760,14 +8767,14 @@
         <v>4.5</v>
       </c>
       <c r="M537" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.2323919403474466</v>
       </c>
       <c r="N537" s="1">
         <v>21</v>
       </c>
       <c r="O537" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>99.771140766215396</v>
       </c>
     </row>
@@ -8776,17 +8783,19 @@
         <v>1802</v>
       </c>
       <c r="B538" s="1">
+        <f t="shared" si="48"/>
+        <v>472.88585565558458</v>
+      </c>
+      <c r="C538" s="1">
         <f t="shared" si="45"/>
-        <v>472.88585565558458</v>
-      </c>
-      <c r="C538" s="1">
-        <f t="shared" si="46"/>
         <v>677.89079723277416</v>
       </c>
       <c r="D538" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>101.68361958491612</v>
       </c>
+      <c r="E538" s="16"/>
+      <c r="F538" s="16"/>
       <c r="H538" s="1">
         <v>0</v>
       </c>
@@ -8797,14 +8806,14 @@
         <v>4.5</v>
       </c>
       <c r="M538" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.2447158597509214</v>
       </c>
       <c r="N538" s="1">
         <v>22</v>
       </c>
       <c r="O538" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>100.76885217387756</v>
       </c>
     </row>
@@ -8813,27 +8822,27 @@
         <v>1803</v>
       </c>
       <c r="B539" s="1">
+        <f t="shared" si="48"/>
+        <v>9194.0832485837018</v>
+      </c>
+      <c r="C539" s="1">
         <f t="shared" si="45"/>
-        <v>9194.0832485837018</v>
-      </c>
-      <c r="C539" s="1">
-        <f t="shared" si="46"/>
         <v>13179.89182519821</v>
       </c>
       <c r="D539" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>1976.9837737797316</v>
       </c>
-      <c r="E539" s="1">
-        <f t="shared" si="48"/>
+      <c r="E539" s="16">
+        <f t="shared" si="50"/>
         <v>68.274214409810554</v>
       </c>
-      <c r="F539" s="1">
-        <f t="shared" si="49"/>
+      <c r="F539" s="16">
+        <f t="shared" si="51"/>
         <v>72.474454362467057</v>
       </c>
       <c r="H539" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>15156.875598977942</v>
       </c>
       <c r="K539" s="1">
@@ -8843,14 +8852,14 @@
         <v>4.5</v>
       </c>
       <c r="M539" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.2571630183484304</v>
       </c>
       <c r="N539" s="1">
         <v>23</v>
       </c>
       <c r="O539" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>101.77654069561632</v>
       </c>
     </row>
@@ -8859,41 +8868,41 @@
         <v>1804</v>
       </c>
       <c r="B540" s="1">
+        <f t="shared" si="48"/>
+        <v>4341.517752188357</v>
+      </c>
+      <c r="C540" s="1">
         <f t="shared" si="45"/>
-        <v>4341.517752188357</v>
-      </c>
-      <c r="C540" s="1">
-        <f t="shared" si="46"/>
         <v>6223.6476203143775</v>
       </c>
       <c r="D540" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>933.54714304715662</v>
       </c>
-      <c r="E540" s="1">
-        <f t="shared" si="48"/>
+      <c r="E540" s="16">
+        <f t="shared" si="50"/>
         <v>18.494043316179678</v>
       </c>
-      <c r="F540" s="1">
-        <f t="shared" si="49"/>
+      <c r="F540" s="16">
+        <f t="shared" si="51"/>
         <v>19.828117642674595</v>
       </c>
       <c r="H540" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>7157.1947633615346</v>
       </c>
       <c r="L540" s="12">
         <v>4.5</v>
       </c>
       <c r="M540" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.269734648531915</v>
       </c>
       <c r="N540" s="1">
         <v>24</v>
       </c>
       <c r="O540" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>102.79430610257251</v>
       </c>
     </row>
@@ -8902,41 +8911,41 @@
         <v>1805</v>
       </c>
       <c r="B541" s="1">
+        <f t="shared" si="48"/>
+        <v>3654.1107747585343</v>
+      </c>
+      <c r="C541" s="1">
         <f t="shared" si="45"/>
-        <v>3654.1107747585343</v>
-      </c>
-      <c r="C541" s="1">
-        <f t="shared" si="46"/>
         <v>5238.2367470979352</v>
       </c>
       <c r="D541" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>785.73551206469028</v>
       </c>
-      <c r="E541" s="1">
-        <f t="shared" si="48"/>
+      <c r="E541" s="16">
+        <f t="shared" si="50"/>
         <v>11.881602089078156</v>
       </c>
-      <c r="F541" s="1">
-        <f t="shared" si="49"/>
+      <c r="F541" s="16">
+        <f t="shared" si="51"/>
         <v>12.866072495762889</v>
       </c>
       <c r="H541" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>6023.9722591626251</v>
       </c>
       <c r="L541" s="12">
         <v>4.5</v>
       </c>
       <c r="M541" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.2824319950172343</v>
       </c>
       <c r="N541" s="1">
         <v>25</v>
       </c>
       <c r="O541" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>103.82224916359824</v>
       </c>
     </row>
@@ -8945,41 +8954,41 @@
         <v>1806</v>
       </c>
       <c r="B542" s="1">
+        <f t="shared" si="48"/>
+        <v>7258.2820355953681</v>
+      </c>
+      <c r="C542" s="1">
         <f t="shared" si="45"/>
-        <v>7258.2820355953681</v>
-      </c>
-      <c r="C542" s="1">
-        <f t="shared" si="46"/>
         <v>10404.884258652197</v>
       </c>
       <c r="D542" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>1560.7326387978294</v>
       </c>
-      <c r="E542" s="1">
-        <f t="shared" si="48"/>
+      <c r="E542" s="16">
+        <f t="shared" si="50"/>
         <v>23.055138530732229</v>
       </c>
-      <c r="F542" s="1">
-        <f t="shared" si="49"/>
+      <c r="F542" s="16">
+        <f t="shared" si="51"/>
         <v>25.215065470759598</v>
       </c>
       <c r="H542" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>11965.616897450027</v>
       </c>
       <c r="L542" s="12">
         <v>4.5</v>
       </c>
       <c r="M542" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.2952563149674066</v>
       </c>
       <c r="N542" s="1">
         <v>26</v>
       </c>
       <c r="O542" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>104.86047165523422</v>
       </c>
     </row>
@@ -8988,41 +8997,41 @@
         <v>1807</v>
       </c>
       <c r="B543" s="1">
+        <f t="shared" si="48"/>
+        <v>11928.186884259772</v>
+      </c>
+      <c r="C543" s="1">
         <f t="shared" si="45"/>
-        <v>11928.186884259772</v>
-      </c>
-      <c r="C543" s="1">
-        <f t="shared" si="46"/>
         <v>17099.280978286723</v>
       </c>
       <c r="D543" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>2564.8921467430082</v>
       </c>
-      <c r="E543" s="1">
-        <f t="shared" si="48"/>
+      <c r="E543" s="16">
+        <f t="shared" si="50"/>
         <v>35.177411672682879</v>
       </c>
-      <c r="F543" s="1">
-        <f t="shared" si="49"/>
+      <c r="F543" s="16">
+        <f t="shared" si="51"/>
         <v>38.85774724834387</v>
       </c>
       <c r="H543" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>19664.173125029731</v>
       </c>
       <c r="L543" s="12">
         <v>4.5</v>
       </c>
       <c r="M543" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.3082088781170802</v>
       </c>
       <c r="N543" s="1">
         <v>27</v>
       </c>
       <c r="O543" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>105.90907637178653</v>
       </c>
     </row>
@@ -9031,41 +9040,41 @@
         <v>1808</v>
       </c>
       <c r="B544" s="1">
+        <f t="shared" si="48"/>
+        <v>19075.158859078758</v>
+      </c>
+      <c r="C544" s="1">
         <f t="shared" si="45"/>
-        <v>19075.158859078758</v>
-      </c>
-      <c r="C544" s="1">
-        <f t="shared" si="46"/>
         <v>27344.600164443524</v>
       </c>
       <c r="D544" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>4101.6900246665282</v>
       </c>
-      <c r="E544" s="1">
-        <f t="shared" si="48"/>
+      <c r="E544" s="16">
+        <f t="shared" si="50"/>
         <v>67.049659251833802</v>
       </c>
-      <c r="F544" s="1">
-        <f t="shared" si="49"/>
+      <c r="F544" s="16">
+        <f t="shared" si="51"/>
         <v>74.80518248196627</v>
       </c>
       <c r="H544" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>31446.290189110052</v>
       </c>
       <c r="L544" s="12">
         <v>4.5</v>
       </c>
       <c r="M544" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.3212909668982511</v>
       </c>
       <c r="N544" s="1">
         <v>28</v>
       </c>
       <c r="O544" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>106.9681671355044</v>
       </c>
     </row>
@@ -9074,41 +9083,41 @@
         <v>1809</v>
       </c>
       <c r="B545" s="1">
+        <f t="shared" si="48"/>
+        <v>21293.901021108442</v>
+      </c>
+      <c r="C545" s="1">
         <f t="shared" si="45"/>
-        <v>21293.901021108442</v>
-      </c>
-      <c r="C545" s="1">
-        <f t="shared" si="46"/>
         <v>30525.208920413002</v>
       </c>
       <c r="D545" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>4578.78133806195</v>
       </c>
-      <c r="E545" s="1">
-        <f t="shared" si="48"/>
+      <c r="E545" s="16">
+        <f t="shared" si="50"/>
         <v>61.478091520971894</v>
       </c>
-      <c r="F545" s="1">
-        <f t="shared" si="49"/>
+      <c r="F545" s="16">
+        <f t="shared" si="51"/>
         <v>69.275052330575136</v>
       </c>
       <c r="H545" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>35103.990258474951</v>
       </c>
       <c r="L545" s="12">
         <v>4.5</v>
       </c>
       <c r="M545" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.3345038765672337</v>
       </c>
       <c r="N545" s="1">
         <v>29</v>
       </c>
       <c r="O545" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>108.03784880685946</v>
       </c>
     </row>
@@ -9117,41 +9126,41 @@
         <v>1810</v>
       </c>
       <c r="B546" s="1">
+        <f t="shared" si="48"/>
+        <v>26883.550039149417</v>
+      </c>
+      <c r="C546" s="1">
         <f t="shared" si="45"/>
-        <v>26883.550039149417</v>
-      </c>
-      <c r="C546" s="1">
-        <f t="shared" si="46"/>
         <v>38538.07626202143</v>
       </c>
       <c r="D546" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>5780.7114393032143</v>
       </c>
-      <c r="E546" s="1">
-        <f t="shared" si="48"/>
+      <c r="E546" s="16">
+        <f t="shared" si="50"/>
         <v>71.597395317164214</v>
       </c>
-      <c r="F546" s="1">
-        <f t="shared" si="49"/>
+      <c r="F546" s="16">
+        <f t="shared" si="51"/>
         <v>81.484514506990465</v>
       </c>
       <c r="H546" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>44318.787701324647</v>
       </c>
       <c r="L546" s="12">
         <v>4.5</v>
       </c>
       <c r="M546" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.3478489153329063</v>
       </c>
       <c r="N546" s="1">
         <v>30</v>
       </c>
       <c r="O546" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>109.11822729492808</v>
       </c>
     </row>
@@ -9160,41 +9169,41 @@
         <v>1811</v>
       </c>
       <c r="B547" s="1">
+        <f t="shared" si="48"/>
+        <v>27928.167983527783</v>
+      </c>
+      <c r="C547" s="1">
         <f t="shared" si="45"/>
-        <v>27928.167983527783</v>
-      </c>
-      <c r="C547" s="1">
-        <f t="shared" si="46"/>
         <v>40035.555796774242</v>
       </c>
       <c r="D547" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>6005.3333695161364</v>
       </c>
-      <c r="E547" s="1">
-        <f t="shared" si="48"/>
+      <c r="E547" s="16">
+        <f t="shared" si="50"/>
         <v>97.959338651681648</v>
       </c>
-      <c r="F547" s="1">
-        <f t="shared" si="49"/>
+      <c r="F547" s="16">
+        <f t="shared" si="51"/>
         <v>112.60173372591954</v>
       </c>
       <c r="H547" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>46040.889166290377</v>
       </c>
       <c r="L547" s="12">
         <v>4.5</v>
       </c>
       <c r="M547" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.3613274044862349</v>
       </c>
       <c r="N547" s="1">
         <v>31</v>
       </c>
       <c r="O547" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>110.20940956787732</v>
       </c>
     </row>
@@ -9203,41 +9212,41 @@
         <v>1812</v>
       </c>
       <c r="B548" s="1">
+        <f t="shared" si="48"/>
+        <v>10969.563757974527</v>
+      </c>
+      <c r="C548" s="1">
         <f t="shared" si="45"/>
-        <v>10969.563757974527</v>
-      </c>
-      <c r="C548" s="1">
-        <f t="shared" si="46"/>
         <v>15725.076637955222</v>
       </c>
       <c r="D548" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>2358.7614956932835</v>
       </c>
-      <c r="E548" s="1">
-        <f t="shared" si="48"/>
+      <c r="E548" s="16">
+        <f t="shared" si="50"/>
         <v>38.071238176102121</v>
       </c>
-      <c r="F548" s="1">
-        <f t="shared" si="49"/>
+      <c r="F548" s="16">
+        <f t="shared" si="51"/>
         <v>44.199525614951696</v>
       </c>
       <c r="H548" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>18083.838133648507</v>
       </c>
       <c r="L548" s="12">
         <v>4.5</v>
       </c>
       <c r="M548" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.3749406785310976</v>
       </c>
       <c r="N548" s="1">
         <v>32</v>
       </c>
       <c r="O548" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>111.31150366355611</v>
       </c>
     </row>
@@ -9246,41 +9255,41 @@
         <v>1813</v>
       </c>
       <c r="B549" s="1">
+        <f t="shared" si="48"/>
+        <v>10155.987779258083</v>
+      </c>
+      <c r="C549" s="1">
         <f t="shared" si="45"/>
-        <v>10155.987779258083</v>
-      </c>
-      <c r="C549" s="1">
-        <f t="shared" si="46"/>
         <v>14558.80012064021</v>
       </c>
       <c r="D549" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>2183.8200180960312</v>
       </c>
-      <c r="E549" s="1">
-        <f t="shared" si="48"/>
+      <c r="E549" s="16">
+        <f t="shared" si="50"/>
         <v>45.128356169100378</v>
       </c>
-      <c r="F549" s="1">
-        <f t="shared" si="49"/>
+      <c r="F549" s="16">
+        <f t="shared" si="51"/>
         <v>52.916546724397762</v>
       </c>
       <c r="H549" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>16742.620138736242</v>
       </c>
       <c r="L549" s="12">
         <v>4.5</v>
       </c>
       <c r="M549" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.3886900853164086</v>
       </c>
       <c r="N549" s="1">
         <v>33</v>
       </c>
       <c r="O549" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="47"/>
         <v>112.42461870019169</v>
       </c>
     </row>
@@ -9289,34 +9298,34 @@
         <v>1814</v>
       </c>
       <c r="B550" s="1">
+        <f t="shared" si="48"/>
+        <v>3330.3726159255402</v>
+      </c>
+      <c r="C550" s="1">
         <f t="shared" si="45"/>
-        <v>3330.3726159255402</v>
-      </c>
-      <c r="C550" s="1">
-        <f t="shared" si="46"/>
         <v>4774.1519876125367</v>
       </c>
       <c r="D550" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>716.12279814188048</v>
       </c>
-      <c r="E550" s="1">
-        <f t="shared" si="48"/>
+      <c r="E550" s="16">
+        <f t="shared" si="50"/>
         <v>37.863964039685634</v>
       </c>
-      <c r="F550" s="1">
-        <f t="shared" si="49"/>
+      <c r="F550" s="16">
+        <f t="shared" si="51"/>
         <v>44.842460401545182</v>
       </c>
       <c r="H550" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>5490.2747857544173</v>
       </c>
       <c r="L550" s="12">
         <v>4.5</v>
       </c>
       <c r="M550" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.4025769861695727</v>
       </c>
       <c r="N550" s="1">
@@ -9336,13 +9345,15 @@
         <v>134.54705368339179</v>
       </c>
       <c r="C551" s="1">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>192.87574029954644</v>
       </c>
       <c r="D551" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>28.931361044931965</v>
       </c>
+      <c r="E551" s="16"/>
+      <c r="F551" s="16"/>
       <c r="H551" s="1">
         <v>0</v>
       </c>
@@ -9350,7 +9361,7 @@
         <v>4.5</v>
       </c>
       <c r="M551" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="46"/>
         <v>1.4166027560312682</v>
       </c>
       <c r="N551" s="1">
@@ -9372,8 +9383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F52ADF-FFA8-0A46-9CC0-C7AD4F73CE98}">
   <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10497,7 +10508,7 @@
         <v>2748.4750941427433</v>
       </c>
       <c r="D108">
-        <f t="shared" ref="D108:D109" si="6">(B108-C108)/C108</f>
+        <f t="shared" ref="D108" si="6">(B108-C108)/C108</f>
         <v>0.43351886956521746</v>
       </c>
       <c r="E108" s="1">

</xml_diff>